<commit_message>
Uplode SahrePointAttachement(upload SharePoint, upload Metadata) ; Process Document (IA classify, Ai Extract, Check invoice Threhold,Invoice Validation)
</commit_message>
<xml_diff>
--- a/Configuration/Config_AR.xlsx
+++ b/Configuration/Config_AR.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="352">
   <si>
     <t>Name</t>
   </si>
@@ -668,6 +668,36 @@
   </si>
   <si>
     <t>Document_confidence</t>
+  </si>
+  <si>
+    <t>SharePointParentFolder</t>
+  </si>
+  <si>
+    <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgAHDSym0Y4OQIWg94J_tGliAenLgaPpG8A1Ae0OItEM6ao?e=uLdM8K</t>
+  </si>
+  <si>
+    <t>SharePointFolder_DSI</t>
+  </si>
+  <si>
+    <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgCMdysN-cJVRJTscSIcJfwIAYAb2Lu0lMUQAZ6-yaJH8vY?e=9PGs0O</t>
+  </si>
+  <si>
+    <t>SharePointFolder_ACHAT</t>
+  </si>
+  <si>
+    <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgCTljwmzmNwTagOpMvdqTmXAcwB8OEiJtqwdd7yPuz56sI?e=FzInGY</t>
+  </si>
+  <si>
+    <t>SharePointFolder_LOG</t>
+  </si>
+  <si>
+    <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgCLpiGYyV_bTrgLo6SYiv52AYs001WXAI7EYue45KdVqmQ?e=UBwrRS</t>
+  </si>
+  <si>
+    <t>SharePointFolder_A_DETERMINER</t>
+  </si>
+  <si>
+    <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgAbdU_t7HW4So2YznO6G_5wAUB7d_upIMseXAUSlG6b6oo?e=ppSRsv</t>
   </si>
   <si>
     <t>Asset_Workday_UI_HomepageURL</t>
@@ -1297,7 +1327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1319,6 +1349,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF828D93"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1493,12 +1535,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,7 +1828,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1816,16 +1852,16 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1834,87 +1870,87 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1981,6 +2017,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2017,7 +2054,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2027,7 +2087,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2064,13 +2124,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2442,216 +2499,216 @@
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4571428571429" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="50.5428571428571" style="32" customWidth="1"/>
-    <col min="2" max="2" width="49.8190476190476" style="33" customWidth="1"/>
-    <col min="3" max="3" width="28.7238095238095" style="33" customWidth="1"/>
-    <col min="4" max="4" width="28.4571428571429" style="33" customWidth="1"/>
-    <col min="5" max="5" width="130.266666666667" style="49" customWidth="1"/>
+    <col min="1" max="1" width="50.5428571428571" style="33" customWidth="1"/>
+    <col min="2" max="2" width="49.8190476190476" style="34" customWidth="1"/>
+    <col min="3" max="3" width="28.7238095238095" style="34" customWidth="1"/>
+    <col min="4" max="4" width="28.4571428571429" style="34" customWidth="1"/>
+    <col min="5" max="5" width="130.266666666667" style="59" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="31" customFormat="1" ht="15.65" customHeight="1" spans="1:5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="15.65" customHeight="1" spans="1:5">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54" t="s">
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="64" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="55" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="65" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="55" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="65" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="56" t="s">
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="66" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="55" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="65" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="55" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="65" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1" spans="2:5">
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68"/>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="55" t="s">
+      <c r="D12" s="41"/>
+      <c r="E12" s="65" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="55" t="s">
+      <c r="D13" s="41"/>
+      <c r="E13" s="65" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="55" t="s">
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="65" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="43"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="44"/>
     </row>
     <row r="16" ht="14.25" customHeight="1" spans="1:5">
       <c r="A16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="40" t="b">
+      <c r="B16" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="55" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="65" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2659,12 +2716,12 @@
       <c r="A17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="55" t="s">
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="65" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2672,172 +2729,172 @@
       <c r="A18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="55"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="65"/>
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:5">
       <c r="A19" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="55"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="65"/>
     </row>
     <row r="20" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
       <c r="A20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="55"/>
-    </row>
-    <row r="21" s="48" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A21" s="61"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="63"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="65"/>
+    </row>
+    <row r="21" s="58" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A21" s="71"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="72"/>
     </row>
     <row r="22" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="62"/>
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A23" s="41"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="55"/>
-    </row>
-    <row r="24" s="48" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A24" s="61"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="63"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="65"/>
+    </row>
+    <row r="24" s="58" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A24" s="71"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="72"/>
     </row>
     <row r="25" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="40" t="b">
+      <c r="B25" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="C25" s="40" t="b">
+      <c r="C25" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="55" t="s">
+      <c r="D25" s="41"/>
+      <c r="E25" s="65" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="65" t="str">
+      <c r="B26" s="74" t="str">
         <f>IF(B9="English",LanguageSettings!$B2,IF(B9="Spanish",LanguageSettings!$D2,LanguageSettings!$C2))</f>
         <v>L’exécution du travail a rencontré une exception système, veuillez consulter le fichier journal et le rapport d’expédition</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="54" t="s">
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="64" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A27" s="66"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
+      <c r="A27" s="75"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
     </row>
     <row r="28" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="52"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
     </row>
     <row r="29" ht="14.25" customHeight="1" spans="1:5">
       <c r="A29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="55" t="s">
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="65" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="42" t="s">
+      <c r="C30" s="76"/>
+      <c r="D30" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="55" t="s">
+      <c r="E30" s="65" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="55" t="s">
+      <c r="B31" s="63"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="65" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="55" t="s">
+      <c r="B32" s="63"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="65" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="55" t="s">
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="65" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2845,138 +2902,138 @@
       <c r="A34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="40" t="b">
+      <c r="B34" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="55" t="s">
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="65" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="55" t="s">
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="65" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="54" t="s">
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="64" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D37" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="E37" s="54" t="s">
+      <c r="E37" s="64" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="65">
+      <c r="B38" s="74">
         <v>25</v>
       </c>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="54" t="s">
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="64" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="54"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="64"/>
     </row>
     <row r="40" ht="13.9" customHeight="1" spans="1:4">
-      <c r="A40" s="46"/>
-      <c r="D40" s="57"/>
+      <c r="A40" s="56"/>
+      <c r="D40" s="67"/>
     </row>
     <row r="41" ht="15.65" customHeight="1" spans="1:5">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="55"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="65"/>
     </row>
     <row r="42" ht="13.9" customHeight="1" spans="1:5">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="55" t="s">
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="65" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="43" ht="13.9" customHeight="1" spans="1:4">
-      <c r="A43" s="46"/>
-      <c r="D43" s="57"/>
+      <c r="A43" s="56"/>
+      <c r="D43" s="67"/>
     </row>
     <row r="44" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="40" t="b">
+      <c r="B44" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="C44" s="40" t="b">
+      <c r="C44" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="D44" s="40"/>
-      <c r="E44" s="54"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="64"/>
     </row>
     <row r="45" ht="14.25" customHeight="1" spans="1:5">
       <c r="A45" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="42" t="str">
+      <c r="B45" s="43" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B3,IF(B9="Spanish",LanguageSettings!$D3,LanguageSettings!$C3)),"%ProcessName%",B3)</f>
         <v>189_HR_Workday_Casiers_Judiciaires - Status Report</v>
       </c>
-      <c r="C45" s="42" t="str">
+      <c r="C45" s="43" t="str">
         <f>"DEV - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B3,IF(B9="Spanish",LanguageSettings!$D3,LanguageSettings!$C3)),"%ProcessName%",B3)</f>
         <v>DEV - 189_HR_Workday_Casiers_Judiciaires - Status Report</v>
       </c>
-      <c r="D45" s="42" t="str">
+      <c r="D45" s="43" t="str">
         <f>"INT - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B3,IF(B9="Spanish",LanguageSettings!$D3,LanguageSettings!$C3)),"%ProcessName%",B3)</f>
         <v>INT - 189_HR_Workday_Casiers_Judiciaires - Status Report</v>
       </c>
-      <c r="E45" s="54" t="s">
+      <c r="E45" s="64" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2984,14 +3041,14 @@
       <c r="A46" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="42" t="str">
+      <c r="B46" s="43" t="str">
         <f>IF(B9="English",LanguageSettings!$B4,IF(B9="Spanish",LanguageSettings!$D4,LanguageSettings!$C4))</f>
         <v>&lt;p&gt;Vous trouverez le rapport de dispatch joint à ce mail. 
 %SRSummary%&lt;/p&gt;</v>
       </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="54" t="s">
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="64" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2999,13 +3056,13 @@
       <c r="A47" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="42" t="str">
+      <c r="B47" s="43" t="str">
         <f>IF(B9="English",LanguageSettings!$B5,IF(B9="Spanish",LanguageSettings!$D5,LanguageSettings!$C5))</f>
         <v>&lt;p&gt;Le processus s’est arrêté après avoir atteint le nombre maximum d’erreurs inattendues autorisées. Vous trouverez le rapport de dispatch joint à ce mail.&lt;/p&gt;</v>
       </c>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="54" t="s">
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="64" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3013,13 +3070,13 @@
       <c r="A48" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="43" t="str">
         <f>IF(B9="English",LanguageSettings!$B6,IF(B9="Spanish",LanguageSettings!$D6,LanguageSettings!$C6))</f>
         <v>&lt;p&gt;Résumé : &lt;br&gt;Au total, {0} Transaction(s) ont été traitées. {1} Transaction(s) ont réussi et {2} Transaction(s) n’ont pas réussi. &lt;br&gt;&lt;br&gt;Anomalies : {3}&lt;/p&gt;</v>
       </c>
-      <c r="C48" s="67"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="54" t="s">
+      <c r="C48" s="76"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="64" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3027,30 +3084,30 @@
       <c r="A49" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B49" s="42" t="str">
+      <c r="B49" s="43" t="str">
         <f>IF(B9="English",LanguageSettings!$B7,IF(B9="Spanish",LanguageSettings!$D7,LanguageSettings!$C7))</f>
         <v>&lt;p&gt;Résumé : &lt;br&gt;Aucune donnée de transaction n’a été trouvée. Veuillez vérifier le processus pour plus de détails.&lt;/p&gt;</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="54" t="s">
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="64" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C50" s="45" t="s">
+      <c r="C50" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="D50" s="42" t="s">
+      <c r="D50" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E50" s="55" t="s">
+      <c r="E50" s="65" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3058,12 +3115,12 @@
       <c r="A51" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="54" t="s">
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="64" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3071,10 +3128,10 @@
       <c r="A52" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="42"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="54" t="s">
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="64" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3082,32 +3139,32 @@
       <c r="A53" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="42">
+      <c r="B53" s="43">
         <v>3</v>
       </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="54" t="s">
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="64" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="54" ht="14.25" customHeight="1" spans="1:5">
       <c r="A54" s="10"/>
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="54"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="64"/>
     </row>
     <row r="55" ht="14.25" customHeight="1" spans="1:5">
       <c r="A55" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="42"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="54" t="s">
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="64" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3115,12 +3172,12 @@
       <c r="A56" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="42"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="54" t="s">
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="64" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3128,12 +3185,12 @@
       <c r="A57" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="C57" s="42"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="54" t="s">
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="64" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3141,12 +3198,12 @@
       <c r="A58" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="40" t="b">
+      <c r="B58" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="54" t="s">
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="64" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3154,52 +3211,52 @@
       <c r="A59" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C59" s="42"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="54" t="s">
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="64" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A60" s="66"/>
-      <c r="B60" s="70"/>
-      <c r="C60" s="70"/>
-      <c r="D60" s="70"/>
-      <c r="E60" s="71"/>
+      <c r="A60" s="75"/>
+      <c r="B60" s="79"/>
+      <c r="C60" s="79"/>
+      <c r="D60" s="79"/>
+      <c r="E60" s="80"/>
     </row>
     <row r="61" ht="14.25" customHeight="1" spans="1:5">
       <c r="A61" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="40" t="b">
+      <c r="B61" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="C61" s="40" t="b">
+      <c r="C61" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="D61" s="40"/>
-      <c r="E61" s="54"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="64"/>
     </row>
     <row r="62" ht="14.25" customHeight="1" spans="1:5">
       <c r="A62" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="42" t="str">
+      <c r="B62" s="43" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B10,IF(B9="Spanish",LanguageSettings!$D10,LanguageSettings!$C10)),"%ProcessName%",B3)</f>
         <v>189_HR_Workday_Casiers_Judiciaires - System Exception</v>
       </c>
-      <c r="C62" s="42" t="str">
+      <c r="C62" s="43" t="str">
         <f>"DEV - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B10,IF(B9="Spanish",LanguageSettings!$D10,LanguageSettings!$C10)),"%ProcessName%",B3)</f>
         <v>DEV - 189_HR_Workday_Casiers_Judiciaires - System Exception</v>
       </c>
-      <c r="D62" s="42" t="str">
+      <c r="D62" s="43" t="str">
         <f>"INT - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B10,IF(B9="Spanish",LanguageSettings!$D10,LanguageSettings!$C10)),"%ProcessName%",B3)</f>
         <v>INT - 189_HR_Workday_Casiers_Judiciaires - System Exception</v>
       </c>
-      <c r="E62" s="55" t="s">
+      <c r="E62" s="65" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3207,45 +3264,45 @@
       <c r="A63" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="42" t="str">
+      <c r="B63" s="43" t="str">
         <f>IF(B9="English",LanguageSettings!$B11,IF(B9="Spanish",LanguageSettings!$D11,LanguageSettings!$C11))</f>
         <v>&lt;p&gt;Le %Process% a été interrompu en raison d’une erreur inattendue lors de l’étape d’initialisation. Veuillez informer votre personne de contact RPA.&lt;/p&gt; </v>
       </c>
-      <c r="C63" s="42"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="55" t="s">
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="65" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="64" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="42" t="str">
+      <c r="B64" s="43" t="str">
         <f>IF(B9="English",LanguageSettings!$B12,IF(B9="Spanish",LanguageSettings!$D12,LanguageSettings!$C12))</f>
         <v>&lt;p&gt;La transaction avec l’ID %ID% , avec le collaborateur
  %COLLABORATEUR% , a été interrompue, en raison d’une erreur inattendue. Une capture d’écran et un fichier journal sont joints à ce courrier. Le processus se poursuivra avec la prochaine transaction. Vous recevrez un rapport d’état lorsque toutes les transactions seront traitées. &lt;p&gt;Message - Détails du processus:&lt;br /&gt;%ErrorMessage%&lt;/p&gt; &lt;p&gt;Message - Source de l’activité:&lt;br /&gt;%ErrorSource%&lt;/p&gt; &lt;/p&gt;</v>
       </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="55" t="s">
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="65" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A65" s="41" t="s">
+      <c r="A65" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C65" s="45" t="s">
+      <c r="C65" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="42" t="s">
+      <c r="D65" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E65" s="55" t="s">
+      <c r="E65" s="65" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3253,12 +3310,12 @@
       <c r="A66" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="C66" s="72"/>
-      <c r="D66" s="72"/>
-      <c r="E66" s="55" t="s">
+      <c r="C66" s="81"/>
+      <c r="D66" s="81"/>
+      <c r="E66" s="65" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3266,92 +3323,92 @@
       <c r="A67" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="72"/>
-      <c r="C67" s="72"/>
-      <c r="D67" s="72"/>
-      <c r="E67" s="55" t="s">
+      <c r="B67" s="81"/>
+      <c r="C67" s="81"/>
+      <c r="D67" s="81"/>
+      <c r="E67" s="65" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1" spans="1:4">
-      <c r="A68" s="66"/>
-      <c r="B68" s="57"/>
-      <c r="C68" s="57"/>
-      <c r="D68" s="57"/>
+      <c r="A68" s="75"/>
+      <c r="B68" s="67"/>
+      <c r="C68" s="67"/>
+      <c r="D68" s="67"/>
     </row>
     <row r="69" ht="14.25" customHeight="1" spans="1:5">
       <c r="A69" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B69" s="40" t="b">
+      <c r="B69" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="C69" s="40" t="b">
+      <c r="C69" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="D69" s="40"/>
-      <c r="E69" s="55"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="65"/>
     </row>
     <row r="70" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="B70" s="42" t="str">
+      <c r="B70" s="43" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B13,IF(B9="Spanish",LanguageSettings!$D13,LanguageSettings!$C13)),"%ProcessName%",B3)</f>
         <v>189_HR_Workday_Casiers_Judiciaires - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
       </c>
-      <c r="C70" s="42" t="str">
+      <c r="C70" s="43" t="str">
         <f>"DEV - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B13,IF(B9="Spanish",LanguageSettings!$D13,LanguageSettings!$C13)),"%ProcessName%",B3)</f>
         <v>DEV - 189_HR_Workday_Casiers_Judiciaires - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
       </c>
-      <c r="D70" s="42" t="str">
+      <c r="D70" s="43" t="str">
         <f>"INT - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B13,IF(B9="Spanish",LanguageSettings!$D13,LanguageSettings!$C13)),"%ProcessName%",B3)</f>
         <v>INT - 189_HR_Workday_Casiers_Judiciaires - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
       </c>
-      <c r="E70" s="55" t="s">
+      <c r="E70" s="65" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A71" s="41" t="s">
+      <c r="A71" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="B71" s="53" t="str">
+      <c r="B71" s="63" t="str">
         <f>IF(B9="English",LanguageSettings!$B14,IF(B9="Spanish",LanguageSettings!$D14,LanguageSettings!$C14))</f>
         <v>&lt;p&gt;La transaction avec l’ID %ID% , avec le collaborateur
  %COLLABORATEUR% ,  a été interrompue, en raison d’une erreur définie. Le processus se poursuivra avec la prochaine transaction. Vous recevrez un rapport d’état lorsque toutes les transactions seront traitées. &lt;p&gt;Cause de l’erreur:&lt;br /&gt;%ErrorMessage%&lt;/p&gt;&lt;/p&gt;</v>
       </c>
-      <c r="C71" s="53"/>
-      <c r="D71" s="53"/>
-      <c r="E71" s="55"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="65"/>
     </row>
     <row r="72" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C72" s="45" t="s">
+      <c r="C72" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="D72" s="42" t="s">
+      <c r="D72" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E72" s="55" t="s">
+      <c r="E72" s="65" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A73" s="41" t="s">
+      <c r="A73" s="42" t="s">
         <v>139</v>
       </c>
       <c r="B73" t="s">
         <v>140</v>
       </c>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40"/>
-      <c r="E73" s="55" t="s">
+      <c r="C73" s="41"/>
+      <c r="D73" s="41"/>
+      <c r="E73" s="65" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3359,96 +3416,96 @@
       <c r="A74" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="55" t="s">
+      <c r="B74" s="41"/>
+      <c r="C74" s="41"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="65" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A75" s="73"/>
-      <c r="B75" s="47"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="74"/>
+      <c r="A75" s="82"/>
+      <c r="B75" s="57"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="83"/>
     </row>
     <row r="76" ht="14.25" customHeight="1" spans="1:5">
       <c r="A76" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="40" t="b">
+      <c r="B76" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="C76" s="40" t="b">
+      <c r="C76" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="D76" s="40"/>
-      <c r="E76" s="55" t="s">
+      <c r="D76" s="41"/>
+      <c r="E76" s="65" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="42" t="str">
+      <c r="B77" s="43" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B8,IF(B9="Spanish",LanguageSettings!$D8,LanguageSettings!$C8)),"%Process%",B3)</f>
         <v>189_HR_Workday_Casiers_Judiciaires - Process Started</v>
       </c>
-      <c r="C77" s="42" t="str">
+      <c r="C77" s="43" t="str">
         <f>"DEV - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B8,IF(B9="Spanish",LanguageSettings!$D8,LanguageSettings!$C8)),"%Process%",B3)</f>
         <v>DEV - 189_HR_Workday_Casiers_Judiciaires - Process Started</v>
       </c>
-      <c r="D77" s="42" t="str">
+      <c r="D77" s="43" t="str">
         <f>"INT - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B8,IF(B9="Spanish",LanguageSettings!$D8,LanguageSettings!$C8)),"%Process%",B3)</f>
         <v>INT - 189_HR_Workday_Casiers_Judiciaires - Process Started</v>
       </c>
-      <c r="E77" s="55" t="s">
+      <c r="E77" s="65" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="78" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A78" s="41" t="s">
+      <c r="A78" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="42" t="str">
+      <c r="B78" s="43" t="str">
         <f>IF(B9="English",LanguageSettings!$B9,IF(B9="Spanish",LanguageSettings!$D9,LanguageSettings!$C9))</f>
         <v>&lt;p&gt;Le processus d’exécution a démarré avec succès et va maintenant commencer à traiter les éléments de travail dans la file d’attente (s’il y en a).&lt;/p&gt;</v>
       </c>
-      <c r="C78" s="53"/>
-      <c r="D78" s="53"/>
-      <c r="E78" s="55" t="s">
+      <c r="C78" s="63"/>
+      <c r="D78" s="63"/>
+      <c r="E78" s="65" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="79" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="42" t="s">
+      <c r="B79" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C79" s="45" t="s">
+      <c r="C79" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="D79" s="42" t="s">
+      <c r="D79" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E79" s="55" t="s">
+      <c r="E79" s="65" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="42" t="s">
         <v>152</v>
       </c>
       <c r="B80" t="s">
         <v>100</v>
       </c>
-      <c r="C80" s="40"/>
-      <c r="D80" s="40"/>
-      <c r="E80" s="55" t="s">
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="65" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3456,18 +3513,18 @@
       <c r="A81" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B81" s="42"/>
-      <c r="C81" s="40"/>
-      <c r="D81" s="40"/>
-      <c r="E81" s="55" t="s">
+      <c r="B81" s="43"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="65" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="82" s="32" customFormat="1" ht="14.25" customHeight="1" spans="2:5">
-      <c r="B82" s="33"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="49"/>
+    <row r="82" s="33" customFormat="1" ht="14.25" customHeight="1" spans="2:5">
+      <c r="B82" s="34"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3508,34 +3565,34 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4571428571429" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41.1809523809524" style="32" customWidth="1"/>
-    <col min="2" max="2" width="112.266666666667" style="33" customWidth="1"/>
-    <col min="3" max="3" width="30.3619047619048" style="33" customWidth="1"/>
-    <col min="4" max="4" width="36.7238095238095" style="33" customWidth="1"/>
-    <col min="5" max="5" width="214.266666666667" style="34" customWidth="1"/>
+    <col min="1" max="1" width="41.1809523809524" style="33" customWidth="1"/>
+    <col min="2" max="2" width="112.266666666667" style="34" customWidth="1"/>
+    <col min="3" max="3" width="30.3619047619048" style="34" customWidth="1"/>
+    <col min="4" max="4" width="36.7238095238095" style="34" customWidth="1"/>
+    <col min="5" max="5" width="214.266666666667" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="31" customFormat="1" ht="15.65" customHeight="1" spans="1:5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
@@ -3543,719 +3600,791 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:14">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="39" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:14">
       <c r="A3" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="39" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:14">
       <c r="A4" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:14">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:14">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:14">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="42" t="s">
         <v>166</v>
       </c>
       <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="43"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="44"/>
     </row>
     <row r="10" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="41" t="s">
         <v>175</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="E10" s="43"/>
+      <c r="E10" s="44"/>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="43"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="43"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="44"/>
     </row>
     <row r="13" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="44"/>
     </row>
     <row r="14" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="44" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="44"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="43"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="44"/>
     </row>
     <row r="18" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="45">
         <v>20</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="43"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="43"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="44"/>
     </row>
     <row r="20" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="43"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="44"/>
     </row>
     <row r="21" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="41" t="s">
         <v>198</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="43"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="44"/>
     </row>
     <row r="22" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="43"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="44"/>
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="43"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="44"/>
     </row>
     <row r="24" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="D24" s="40"/>
-      <c r="E24" s="43"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="43"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="44"/>
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="43"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="44"/>
     </row>
     <row r="27" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="44">
+      <c r="B27" s="48">
         <v>0.5</v>
       </c>
-      <c r="C27" s="44">
+      <c r="C27" s="49">
         <v>0.5</v>
       </c>
-      <c r="D27" s="40"/>
-      <c r="E27" s="43"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="44"/>
+    </row>
+    <row r="28" s="32" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="53"/>
     </row>
     <row r="29" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="43"/>
+      <c r="C29" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D29" s="41"/>
+      <c r="E29" s="44"/>
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="43"/>
+      <c r="C30" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="D30" s="41"/>
+      <c r="E30" s="44"/>
     </row>
     <row r="31" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="43"/>
+      <c r="C31" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="D31" s="41"/>
+      <c r="E31" s="44"/>
     </row>
     <row r="32" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A32" s="41"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="43"/>
+      <c r="A32" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="D32" s="41"/>
+      <c r="E32" s="44"/>
     </row>
     <row r="33" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A33" s="41" t="s">
-        <v>216</v>
-      </c>
-      <c r="B33" s="40" t="s">
+      <c r="A33" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" s="41"/>
+      <c r="E33" s="44"/>
+    </row>
+    <row r="35" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A35" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="44"/>
+    </row>
+    <row r="36" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A36" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="44"/>
+    </row>
+    <row r="37" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A37" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="44"/>
+    </row>
+    <row r="38" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A38" s="42"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="44"/>
+    </row>
+    <row r="39" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A39" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="B39" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C39" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D39" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="E33" s="43"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A34" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="45" t="s">
+      <c r="E39" s="44"/>
+    </row>
+    <row r="40" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A40" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="41"/>
+      <c r="C40" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D40" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="E34" s="43"/>
-    </row>
-    <row r="35" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A35" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="B35" s="40" t="s">
-        <v>219</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>219</v>
-      </c>
-      <c r="D35" s="40" t="s">
-        <v>219</v>
-      </c>
-      <c r="E35" s="43"/>
-    </row>
-    <row r="36" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A36" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="B36" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="D36" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="E36" s="43"/>
-    </row>
-    <row r="37" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A37" s="41" t="s">
-        <v>222</v>
-      </c>
-      <c r="B37" s="40" t="s">
-        <v>223</v>
-      </c>
-      <c r="C37" s="40" t="s">
-        <v>224</v>
-      </c>
-      <c r="D37" s="40" t="s">
-        <v>225</v>
-      </c>
-      <c r="E37" s="43"/>
-    </row>
-    <row r="38" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A38" s="41"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="43"/>
-    </row>
-    <row r="39" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A39" s="41"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="43"/>
-    </row>
-    <row r="40" customHeight="1" spans="1:4">
-      <c r="A40" s="46"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-    </row>
-    <row r="41" customHeight="1" spans="1:4">
-      <c r="A41" s="46"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-    </row>
-    <row r="42" customHeight="1" spans="1:4">
-      <c r="A42" s="46"/>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-    </row>
-    <row r="43" customHeight="1" spans="1:4">
-      <c r="A43" s="46"/>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-    </row>
-    <row r="44" customHeight="1" spans="1:4">
-      <c r="A44" s="46"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-    </row>
-    <row r="45" customHeight="1" spans="1:4">
-      <c r="A45" s="46"/>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
+      <c r="E40" s="44"/>
+    </row>
+    <row r="41" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A41" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="D41" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="E41" s="44"/>
+    </row>
+    <row r="42" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A42" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="B42" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="D42" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="E42" s="44"/>
+    </row>
+    <row r="43" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A43" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>233</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" s="44"/>
+    </row>
+    <row r="44" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A44" s="42"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="44"/>
+    </row>
+    <row r="45" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A45" s="42"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="44"/>
     </row>
     <row r="46" customHeight="1" spans="1:4">
-      <c r="A46" s="46"/>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
+      <c r="A46" s="56"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
     </row>
     <row r="47" customHeight="1" spans="1:4">
-      <c r="A47" s="46"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
+      <c r="A47" s="56"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
     </row>
     <row r="48" customHeight="1" spans="1:4">
-      <c r="A48" s="46"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
+      <c r="A48" s="56"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
     </row>
     <row r="49" customHeight="1" spans="1:4">
-      <c r="A49" s="46"/>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
+      <c r="A49" s="56"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
     </row>
     <row r="50" customHeight="1" spans="1:4">
-      <c r="A50" s="46"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
+      <c r="A50" s="56"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
     </row>
     <row r="51" customHeight="1" spans="1:4">
-      <c r="A51" s="46"/>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
+      <c r="A51" s="56"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
     </row>
     <row r="52" customHeight="1" spans="1:4">
-      <c r="A52" s="46"/>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
+      <c r="A52" s="56"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
     </row>
     <row r="53" customHeight="1" spans="1:4">
-      <c r="A53" s="46"/>
-      <c r="B53" s="47"/>
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
+      <c r="A53" s="56"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
     </row>
     <row r="54" customHeight="1" spans="1:4">
-      <c r="A54" s="46"/>
-      <c r="B54" s="47"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="47"/>
+      <c r="A54" s="56"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
     </row>
     <row r="55" customHeight="1" spans="1:4">
-      <c r="A55" s="46"/>
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
+      <c r="A55" s="56"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
     </row>
     <row r="56" customHeight="1" spans="1:4">
-      <c r="A56" s="46"/>
-      <c r="B56" s="47"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
+      <c r="A56" s="56"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="57"/>
     </row>
     <row r="57" customHeight="1" spans="1:4">
-      <c r="A57" s="46"/>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
+      <c r="A57" s="56"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
     </row>
     <row r="58" customHeight="1" spans="1:4">
-      <c r="A58" s="46"/>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
+      <c r="A58" s="56"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
     </row>
     <row r="59" customHeight="1" spans="1:4">
-      <c r="A59" s="46"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
+      <c r="A59" s="56"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
     </row>
     <row r="60" customHeight="1" spans="1:4">
-      <c r="A60" s="46"/>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
+      <c r="A60" s="56"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
     </row>
     <row r="61" customHeight="1" spans="1:4">
-      <c r="A61" s="46"/>
-      <c r="B61" s="47"/>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
+      <c r="A61" s="56"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
     </row>
     <row r="62" customHeight="1" spans="1:4">
-      <c r="A62" s="46"/>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
+      <c r="A62" s="56"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
     </row>
     <row r="63" customHeight="1" spans="1:4">
-      <c r="A63" s="46"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
+      <c r="A63" s="56"/>
+      <c r="B63" s="57"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
     </row>
     <row r="64" customHeight="1" spans="1:4">
-      <c r="A64" s="46"/>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
+      <c r="A64" s="56"/>
+      <c r="B64" s="57"/>
+      <c r="C64" s="57"/>
+      <c r="D64" s="57"/>
     </row>
     <row r="65" customHeight="1" spans="1:4">
-      <c r="A65" s="46"/>
-      <c r="B65" s="47"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
+      <c r="A65" s="56"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
     </row>
     <row r="66" customHeight="1" spans="1:4">
-      <c r="A66" s="46"/>
-      <c r="B66" s="47"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
+      <c r="A66" s="56"/>
+      <c r="B66" s="57"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="57"/>
     </row>
     <row r="67" customHeight="1" spans="1:4">
-      <c r="A67" s="46"/>
-      <c r="B67" s="47"/>
-      <c r="C67" s="47"/>
-      <c r="D67" s="47"/>
+      <c r="A67" s="56"/>
+      <c r="B67" s="57"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57"/>
     </row>
     <row r="68" customHeight="1" spans="1:4">
-      <c r="A68" s="46"/>
-      <c r="B68" s="47"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
+      <c r="A68" s="56"/>
+      <c r="B68" s="57"/>
+      <c r="C68" s="57"/>
+      <c r="D68" s="57"/>
     </row>
     <row r="69" customHeight="1" spans="1:4">
-      <c r="A69" s="46"/>
-      <c r="B69" s="47"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
+      <c r="A69" s="56"/>
+      <c r="B69" s="57"/>
+      <c r="C69" s="57"/>
+      <c r="D69" s="57"/>
     </row>
     <row r="70" customHeight="1" spans="1:4">
-      <c r="A70" s="46"/>
-      <c r="B70" s="47"/>
-      <c r="C70" s="47"/>
-      <c r="D70" s="47"/>
+      <c r="A70" s="56"/>
+      <c r="B70" s="57"/>
+      <c r="C70" s="57"/>
+      <c r="D70" s="57"/>
     </row>
     <row r="71" customHeight="1" spans="1:4">
-      <c r="A71" s="46"/>
-      <c r="B71" s="47"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
+      <c r="A71" s="56"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="57"/>
+      <c r="D71" s="57"/>
     </row>
     <row r="72" customHeight="1" spans="1:4">
-      <c r="A72" s="46"/>
-      <c r="B72" s="47"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
+      <c r="A72" s="56"/>
+      <c r="B72" s="57"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="57"/>
     </row>
     <row r="73" customHeight="1" spans="1:4">
-      <c r="A73" s="46"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
+      <c r="A73" s="56"/>
+      <c r="B73" s="57"/>
+      <c r="C73" s="57"/>
+      <c r="D73" s="57"/>
     </row>
     <row r="74" customHeight="1" spans="1:4">
-      <c r="A74" s="46"/>
-      <c r="B74" s="47"/>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
+      <c r="A74" s="56"/>
+      <c r="B74" s="57"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
     </row>
     <row r="75" customHeight="1" spans="1:4">
-      <c r="A75" s="46"/>
-      <c r="B75" s="47"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
+      <c r="A75" s="56"/>
+      <c r="B75" s="57"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
+    </row>
+    <row r="76" customHeight="1" spans="1:4">
+      <c r="A76" s="56"/>
+      <c r="B76" s="57"/>
+      <c r="C76" s="57"/>
+      <c r="D76" s="57"/>
+    </row>
+    <row r="77" customHeight="1" spans="1:4">
+      <c r="A77" s="56"/>
+      <c r="B77" s="57"/>
+      <c r="C77" s="57"/>
+      <c r="D77" s="57"/>
+    </row>
+    <row r="78" customHeight="1" spans="1:4">
+      <c r="A78" s="56"/>
+      <c r="B78" s="57"/>
+      <c r="C78" s="57"/>
+      <c r="D78" s="57"/>
+    </row>
+    <row r="79" customHeight="1" spans="1:4">
+      <c r="A79" s="56"/>
+      <c r="B79" s="57"/>
+      <c r="C79" s="57"/>
+      <c r="D79" s="57"/>
+    </row>
+    <row r="80" customHeight="1" spans="1:4">
+      <c r="A80" s="56"/>
+      <c r="B80" s="57"/>
+      <c r="C80" s="57"/>
+      <c r="D80" s="57"/>
+    </row>
+    <row r="81" customHeight="1" spans="1:4">
+      <c r="A81" s="56"/>
+      <c r="B81" s="57"/>
+      <c r="C81" s="57"/>
+      <c r="D81" s="57"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C34" r:id="rId1" display="fkinedieng.ext@fdjunited.com"/>
-    <hyperlink ref="D34" r:id="rId1" display="fkinedieng.ext@fdjunited.com"/>
+    <hyperlink ref="C40" r:id="rId1" display="fkinedieng.ext@fdjunited.com"/>
+    <hyperlink ref="D40" r:id="rId1" display="fkinedieng.ext@fdjunited.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4305,7 +4434,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:5">
       <c r="A2" s="20" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -4314,7 +4443,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:5">
       <c r="A3" s="23" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="B3" s="24">
         <v>0</v>
@@ -4322,12 +4451,12 @@
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="E3" s="25" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:5">
       <c r="A4" s="15" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B4" s="4">
         <v>200</v>
@@ -4335,12 +4464,12 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="14" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:5">
       <c r="A5" s="15" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
@@ -4348,12 +4477,12 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="14" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:5">
       <c r="A6" s="16" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="B6" s="17">
         <v>3</v>
@@ -4361,13 +4490,13 @@
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="18" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1"/>
     <row r="8" ht="14.25" customHeight="1" spans="1:5">
       <c r="A8" s="23" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="B8" s="24">
         <v>5</v>
@@ -4375,12 +4504,12 @@
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
       <c r="E8" s="25" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:5">
       <c r="A9" s="15" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="B9" s="4">
         <v>30</v>
@@ -4388,12 +4517,12 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="14" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1" spans="1:5">
       <c r="A10" s="16" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="B10" s="17">
         <v>120</v>
@@ -4401,13 +4530,13 @@
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1" spans="1:5">
       <c r="A12" s="23" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="B12" s="24">
         <v>1</v>
@@ -4415,12 +4544,12 @@
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
       <c r="E12" s="25" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1" spans="1:5">
       <c r="A13" s="15" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="B13" s="4">
         <v>15</v>
@@ -4428,12 +4557,12 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="14" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1" spans="1:5">
       <c r="A14" s="16" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="B14" s="17">
         <v>60</v>
@@ -4441,13 +4570,13 @@
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
       <c r="E14" s="18" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1"/>
     <row r="16" ht="14.25" customHeight="1" spans="1:5">
       <c r="A16" s="23" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="B16" s="24">
         <v>0.6</v>
@@ -4455,12 +4584,12 @@
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="25" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" spans="1:5">
       <c r="A17" s="15" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="B17" s="4">
         <v>0.8</v>
@@ -4468,12 +4597,12 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="14" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1" spans="1:5">
       <c r="A18" s="16" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="B18" s="17">
         <v>0.9</v>
@@ -4481,92 +4610,92 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="18" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1" spans="1:5">
       <c r="A20" s="23" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="25" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1" spans="1:5">
       <c r="A21" s="15" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="14" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1" spans="1:5">
       <c r="A22" s="15" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="14" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:5">
       <c r="A23" s="15" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="14" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1" spans="1:5">
       <c r="A24" s="16" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="18" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1" spans="1:5">
       <c r="A25" s="16" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="18" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1"/>
     <row r="27" ht="14.25" customHeight="1" spans="1:5">
       <c r="A27" s="23" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="B27" s="24">
         <v>0</v>
@@ -4574,12 +4703,12 @@
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="25" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1" spans="1:5">
       <c r="A28" s="15" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="B28" s="4">
         <v>0</v>
@@ -4587,12 +4716,12 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="14" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1" spans="1:5">
       <c r="A29" s="16" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="B29" s="17">
         <v>0</v>
@@ -4600,30 +4729,30 @@
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="18" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1" spans="1:5">
       <c r="A31" s="23" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" ht="14.15" customHeight="1" spans="1:5">
       <c r="A32" s="16" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="B32" s="17">
         <v>7</v>
@@ -4631,13 +4760,13 @@
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="18" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" ht="14.15" customHeight="1"/>
     <row r="34" ht="14.15" customHeight="1" spans="1:5">
       <c r="A34" s="23" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="B34" s="24">
         <v>3</v>
@@ -4645,12 +4774,12 @@
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="25" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
     </row>
     <row r="35" ht="14.15" customHeight="1" spans="1:5">
       <c r="A35" s="16" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="B35" s="17">
         <v>5</v>
@@ -4658,13 +4787,13 @@
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="18" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1"/>
     <row r="37" ht="14.25" customHeight="1" spans="1:5">
       <c r="A37" s="27" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
@@ -4673,7 +4802,7 @@
     </row>
     <row r="38" s="19" customFormat="1" ht="14.25" customHeight="1" spans="1:1">
       <c r="A38" s="30" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4720,18 +4849,18 @@
         <v>37</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>32</v>
@@ -4741,10 +4870,10 @@
     </row>
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="15" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
@@ -4794,19 +4923,19 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:5">
@@ -4814,16 +4943,16 @@
         <v>52</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" ht="15" spans="1:5">
@@ -4831,10 +4960,10 @@
         <v>86</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -4844,16 +4973,16 @@
         <v>88</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" ht="89.25" customHeight="1" spans="1:5">
@@ -4861,16 +4990,16 @@
         <v>90</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" ht="89.25" customHeight="1" spans="1:5">
@@ -4878,16 +5007,16 @@
         <v>92</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" ht="89.25" customHeight="1" spans="1:5">
@@ -4895,16 +5024,16 @@
         <v>94</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:5">
@@ -4912,23 +5041,23 @@
         <v>146</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" ht="89.25" customHeight="1" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -4938,10 +5067,10 @@
         <v>121</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -4951,16 +5080,16 @@
         <v>123</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" ht="178.9" customHeight="1" spans="1:5">
@@ -4968,16 +5097,16 @@
         <v>125</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" ht="45" spans="1:5">
@@ -4985,10 +5114,10 @@
         <v>134</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -4998,16 +5127,16 @@
         <v>136</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" ht="134.5" customHeight="1" spans="1:5">
@@ -5044,13 +5173,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>55</v>
@@ -5064,15 +5193,15 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>0</v>
@@ -5081,12 +5210,12 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>56</v>
@@ -5094,7 +5223,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save Data in sage
</commit_message>
<xml_diff>
--- a/Configuration/Config_AR.xlsx
+++ b/Configuration/Config_AR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7980" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="7380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="372">
   <si>
     <t>Name</t>
   </si>
@@ -640,13 +640,25 @@
     <t>AnnuaireFileName</t>
   </si>
   <si>
-    <t>Annuaire.xlsx</t>
+    <t>Annuaire Utilisateur.xlsx</t>
+  </si>
+  <si>
+    <t>AnnuaireFileFournisseur</t>
+  </si>
+  <si>
+    <t>Annuaire Fournisseur.xlsx</t>
   </si>
   <si>
     <t>AnnuaireFileUrl</t>
   </si>
   <si>
     <t>https://senyone.sharepoint.com/:x:/s/ServicesRH/EcNvdO692pJDpE007LBfz-4B4wA7J_ulFRarWxCrdjw_0A?e=PuwZaQ</t>
+  </si>
+  <si>
+    <t>AnnuaireFileFournissuerUrl</t>
+  </si>
+  <si>
+    <t>https://senyone.sharepoint.com/:x:/s/ServicesRH/IQD9ptQWYnjNS47vm37Sl0rmAXdHYeMA4oK25WfoeJpzJNw?e=JCNkhL</t>
   </si>
   <si>
     <t>AnnuaireFileRange</t>
@@ -3612,12 +3624,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4571428571429" defaultRowHeight="15" customHeight="1"/>
@@ -3952,10 +3964,10 @@
       <c r="A23" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="41" t="s">
         <v>202</v>
       </c>
       <c r="D23" s="41"/>
@@ -4030,47 +4042,47 @@
       <c r="A29" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="B29" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="C29" s="49">
-        <v>0.5</v>
+      <c r="B29" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>214</v>
       </c>
       <c r="D29" s="41"/>
       <c r="E29" s="44"/>
     </row>
-    <row r="30" s="32" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A30" s="50"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="53"/>
+    <row r="30" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A30" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="B30" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="D30" s="41"/>
+      <c r="E30" s="44"/>
     </row>
     <row r="31" ht="14.25" customHeight="1" spans="1:5">
       <c r="A31" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="B31" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="B31" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="C31" s="49">
+        <v>0.5</v>
       </c>
       <c r="D31" s="41"/>
       <c r="E31" s="44"/>
     </row>
-    <row r="32" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A32" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="B32" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="44"/>
+    <row r="32" s="32" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A32" s="50"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="53"/>
     </row>
     <row r="33" ht="14.25" customHeight="1" spans="1:5">
       <c r="A33" s="42" t="s">
@@ -4111,38 +4123,38 @@
       <c r="D35" s="41"/>
       <c r="E35" s="44"/>
     </row>
-    <row r="36" s="32" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A36" s="50"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="53"/>
+    <row r="36" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A36" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="41"/>
+      <c r="E36" s="44"/>
     </row>
     <row r="37" ht="14.25" customHeight="1" spans="1:5">
       <c r="A37" s="42" t="s">
-        <v>224</v>
-      </c>
-      <c r="B37" s="54" t="s">
-        <v>225</v>
-      </c>
-      <c r="C37" s="54" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>227</v>
       </c>
       <c r="D37" s="41"/>
       <c r="E37" s="44"/>
     </row>
-    <row r="38" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A38" s="42" t="s">
-        <v>226</v>
-      </c>
-      <c r="B38" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="C38" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="44"/>
+    <row r="38" s="32" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A38" s="50"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="53"/>
     </row>
     <row r="39" ht="14.25" customHeight="1" spans="1:5">
       <c r="A39" s="42" t="s">
@@ -4174,21 +4186,21 @@
       <c r="A41" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="B41" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="C41" s="47" t="s">
-        <v>231</v>
+      <c r="B41" s="54" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" s="54" t="s">
+        <v>233</v>
       </c>
       <c r="D41" s="41"/>
       <c r="E41" s="44"/>
     </row>
     <row r="42" ht="14.25" customHeight="1" spans="1:5">
       <c r="A42" s="42" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C42" s="47" t="s">
         <v>235</v>
@@ -4196,27 +4208,31 @@
       <c r="D42" s="41"/>
       <c r="E42" s="44"/>
     </row>
+    <row r="43" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A43" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="D43" s="41"/>
+      <c r="E43" s="44"/>
+    </row>
     <row r="44" ht="14.25" customHeight="1" spans="1:5">
       <c r="A44" s="42" t="s">
-        <v>236</v>
-      </c>
-      <c r="B44" s="41" t="s">
         <v>237</v>
       </c>
-      <c r="C44" s="41"/>
+      <c r="B44" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>239</v>
+      </c>
       <c r="D44" s="41"/>
       <c r="E44" s="44"/>
-    </row>
-    <row r="45" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A45" s="42" t="s">
-        <v>238</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>239</v>
-      </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="44"/>
     </row>
     <row r="46" ht="14.25" customHeight="1" spans="1:5">
       <c r="A46" s="42" t="s">
@@ -4230,67 +4246,59 @@
       <c r="E46" s="44"/>
     </row>
     <row r="47" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A47" s="42"/>
-      <c r="B47" s="41"/>
+      <c r="A47" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="B47" s="41" t="s">
+        <v>243</v>
+      </c>
       <c r="C47" s="41"/>
       <c r="D47" s="41"/>
       <c r="E47" s="44"/>
     </row>
     <row r="48" ht="14.25" customHeight="1" spans="1:5">
       <c r="A48" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B48" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="C48" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="D48" s="41" t="s">
-        <v>157</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
       <c r="E48" s="44"/>
     </row>
     <row r="49" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A49" s="42" t="s">
-        <v>243</v>
-      </c>
+      <c r="A49" s="42"/>
       <c r="B49" s="41"/>
-      <c r="C49" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="55" t="s">
-        <v>97</v>
-      </c>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
       <c r="E49" s="44"/>
     </row>
     <row r="50" ht="14.25" customHeight="1" spans="1:5">
       <c r="A50" s="42" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B50" s="41" t="s">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="C50" s="41" t="s">
-        <v>245</v>
+        <v>157</v>
       </c>
       <c r="D50" s="41" t="s">
-        <v>245</v>
+        <v>157</v>
       </c>
       <c r="E50" s="44"/>
     </row>
     <row r="51" ht="14.25" customHeight="1" spans="1:5">
       <c r="A51" s="42" t="s">
-        <v>246</v>
-      </c>
-      <c r="B51" s="41" t="s">
         <v>247</v>
       </c>
-      <c r="C51" s="41" t="s">
-        <v>247</v>
-      </c>
-      <c r="D51" s="41" t="s">
-        <v>247</v>
+      <c r="B51" s="41"/>
+      <c r="C51" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="55" t="s">
+        <v>97</v>
       </c>
       <c r="E51" s="44"/>
     </row>
@@ -4302,38 +4310,56 @@
         <v>249</v>
       </c>
       <c r="C52" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="E52" s="44"/>
+    </row>
+    <row r="53" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A53" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="D52" s="41" t="s">
+      <c r="B53" s="41" t="s">
         <v>251</v>
       </c>
-      <c r="E52" s="44"/>
-    </row>
-    <row r="53" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A53" s="42"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
+      <c r="C53" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="D53" s="41" t="s">
+        <v>251</v>
+      </c>
       <c r="E53" s="44"/>
     </row>
     <row r="54" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A54" s="42"/>
-      <c r="B54" s="41"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
+      <c r="A54" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="B54" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="C54" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="D54" s="41" t="s">
+        <v>255</v>
+      </c>
       <c r="E54" s="44"/>
     </row>
-    <row r="55" customHeight="1" spans="1:4">
-      <c r="A55" s="56"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-    </row>
-    <row r="56" customHeight="1" spans="1:4">
-      <c r="A56" s="56"/>
-      <c r="B56" s="57"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="57"/>
+    <row r="55" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A55" s="42"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="44"/>
+    </row>
+    <row r="56" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A56" s="42"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="44"/>
     </row>
     <row r="57" customHeight="1" spans="1:4">
       <c r="A57" s="56"/>
@@ -4539,10 +4565,22 @@
       <c r="C90" s="57"/>
       <c r="D90" s="57"/>
     </row>
+    <row r="91" customHeight="1" spans="1:4">
+      <c r="A91" s="56"/>
+      <c r="B91" s="57"/>
+      <c r="C91" s="57"/>
+      <c r="D91" s="57"/>
+    </row>
+    <row r="92" customHeight="1" spans="1:4">
+      <c r="A92" s="56"/>
+      <c r="B92" s="57"/>
+      <c r="C92" s="57"/>
+      <c r="D92" s="57"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C49" r:id="rId1" display="fkinedieng.ext@fdjunited.com"/>
-    <hyperlink ref="D49" r:id="rId1" display="fkinedieng.ext@fdjunited.com"/>
+    <hyperlink ref="C51" r:id="rId1" display="fkinedieng.ext@fdjunited.com"/>
+    <hyperlink ref="D51" r:id="rId1" display="fkinedieng.ext@fdjunited.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4592,7 +4630,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:5">
       <c r="A2" s="20" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -4601,7 +4639,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:5">
       <c r="A3" s="23" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B3" s="24">
         <v>0</v>
@@ -4609,12 +4647,12 @@
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="E3" s="25" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:5">
       <c r="A4" s="15" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B4" s="4">
         <v>200</v>
@@ -4622,12 +4660,12 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="14" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:5">
       <c r="A5" s="15" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
@@ -4635,12 +4673,12 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="14" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:5">
       <c r="A6" s="16" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B6" s="17">
         <v>3</v>
@@ -4648,13 +4686,13 @@
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="18" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1"/>
     <row r="8" ht="14.25" customHeight="1" spans="1:5">
       <c r="A8" s="23" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B8" s="24">
         <v>5</v>
@@ -4662,12 +4700,12 @@
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
       <c r="E8" s="25" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:5">
       <c r="A9" s="15" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B9" s="4">
         <v>30</v>
@@ -4675,12 +4713,12 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="14" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1" spans="1:5">
       <c r="A10" s="16" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B10" s="17">
         <v>120</v>
@@ -4688,13 +4726,13 @@
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1" spans="1:5">
       <c r="A12" s="23" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B12" s="24">
         <v>1</v>
@@ -4702,12 +4740,12 @@
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
       <c r="E12" s="25" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1" spans="1:5">
       <c r="A13" s="15" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B13" s="4">
         <v>15</v>
@@ -4715,12 +4753,12 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="14" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1" spans="1:5">
       <c r="A14" s="16" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B14" s="17">
         <v>60</v>
@@ -4728,13 +4766,13 @@
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
       <c r="E14" s="18" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1"/>
     <row r="16" ht="14.25" customHeight="1" spans="1:5">
       <c r="A16" s="23" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B16" s="24">
         <v>0.6</v>
@@ -4742,12 +4780,12 @@
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="25" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" spans="1:5">
       <c r="A17" s="15" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B17" s="4">
         <v>0.8</v>
@@ -4755,12 +4793,12 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="14" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1" spans="1:5">
       <c r="A18" s="16" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B18" s="17">
         <v>0.9</v>
@@ -4768,92 +4806,92 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="18" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1" spans="1:5">
       <c r="A20" s="23" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="25" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1" spans="1:5">
       <c r="A21" s="15" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="14" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1" spans="1:5">
       <c r="A22" s="15" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="14" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:5">
       <c r="A23" s="15" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="14" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1" spans="1:5">
       <c r="A24" s="16" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="18" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1" spans="1:5">
       <c r="A25" s="16" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="18" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1"/>
     <row r="27" ht="14.25" customHeight="1" spans="1:5">
       <c r="A27" s="23" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B27" s="24">
         <v>0</v>
@@ -4861,12 +4899,12 @@
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="25" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1" spans="1:5">
       <c r="A28" s="15" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B28" s="4">
         <v>0</v>
@@ -4874,12 +4912,12 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="14" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1" spans="1:5">
       <c r="A29" s="16" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B29" s="17">
         <v>0</v>
@@ -4887,30 +4925,30 @@
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="18" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1" spans="1:5">
       <c r="A31" s="23" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" ht="14.15" customHeight="1" spans="1:5">
       <c r="A32" s="16" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B32" s="17">
         <v>7</v>
@@ -4918,13 +4956,13 @@
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="18" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" ht="14.15" customHeight="1"/>
     <row r="34" ht="14.15" customHeight="1" spans="1:5">
       <c r="A34" s="23" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B34" s="24">
         <v>3</v>
@@ -4932,12 +4970,12 @@
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="25" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" ht="14.15" customHeight="1" spans="1:5">
       <c r="A35" s="16" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B35" s="17">
         <v>5</v>
@@ -4945,13 +4983,13 @@
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="18" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1"/>
     <row r="37" ht="14.25" customHeight="1" spans="1:5">
       <c r="A37" s="27" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
@@ -4960,7 +4998,7 @@
     </row>
     <row r="38" s="19" customFormat="1" ht="14.25" customHeight="1" spans="1:1">
       <c r="A38" s="30" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -5007,18 +5045,18 @@
         <v>37</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>32</v>
@@ -5028,10 +5066,10 @@
     </row>
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="15" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
@@ -5081,19 +5119,19 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:5">
@@ -5101,16 +5139,16 @@
         <v>52</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" ht="15" spans="1:5">
@@ -5118,10 +5156,10 @@
         <v>86</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -5131,16 +5169,16 @@
         <v>88</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" ht="89.25" customHeight="1" spans="1:5">
@@ -5148,16 +5186,16 @@
         <v>90</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" ht="89.25" customHeight="1" spans="1:5">
@@ -5165,16 +5203,16 @@
         <v>92</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" ht="89.25" customHeight="1" spans="1:5">
@@ -5182,16 +5220,16 @@
         <v>94</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:5">
@@ -5199,23 +5237,23 @@
         <v>146</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" ht="89.25" customHeight="1" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -5225,10 +5263,10 @@
         <v>121</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -5238,16 +5276,16 @@
         <v>123</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" ht="178.9" customHeight="1" spans="1:5">
@@ -5255,16 +5293,16 @@
         <v>125</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" ht="45" spans="1:5">
@@ -5272,10 +5310,10 @@
         <v>134</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -5285,16 +5323,16 @@
         <v>136</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" ht="134.5" customHeight="1" spans="1:5">
@@ -5331,13 +5369,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>55</v>
@@ -5351,15 +5389,15 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>0</v>
@@ -5368,12 +5406,12 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>56</v>
@@ -5381,7 +5419,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sage invoice enter OK 70 percent done Updata metadata OK Move file to right direction OK
</commit_message>
<xml_diff>
--- a/Configuration/Config_AR.xlsx
+++ b/Configuration/Config_AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\SynologyDrive\UiPath RPA\Studio\0. SENICO\rpa-senico-factures-frs\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Travail\SynologyDrive\Pro\Projets Pro\UiPath RPA\Studio\0. SENICO\rpa-senico-factures-frs\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE9B674-36DE-401B-B0D9-80C295479399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C50F7FD-6B82-46C7-96AC-6D4F11DBBE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8436" yWindow="1212" windowWidth="16440" windowHeight="13836" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="23016" windowHeight="14460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="398">
   <si>
     <t>Name</t>
   </si>
@@ -65,9 +65,6 @@
     <t>ProcessName</t>
   </si>
   <si>
-    <t>189_HR_Workday_Casiers_Judiciaires</t>
-  </si>
-  <si>
     <t>Name of your process. This name appears in Process folders and Mail subject</t>
   </si>
   <si>
@@ -611,9 +608,6 @@
     <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgCMdysN-cJVRJTscSIcJfwIAYAb2Lu0lMUQAZ6-yaJH8vY?e=9PGs0O</t>
   </si>
   <si>
-    <t>SharePointFolder_ACHAT</t>
-  </si>
-  <si>
     <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgCTljwmzmNwTagOpMvdqTmXAcwB8OEiJtqwdd7yPuz56sI?e=FzInGY</t>
   </si>
   <si>
@@ -624,9 +618,6 @@
   </si>
   <si>
     <t>SharePointFolder_A_DETERMINER</t>
-  </si>
-  <si>
-    <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgAbdU_t7HW4So2YznO6G_5wAUB7d_upIMseXAUSlG6b6oo?e=ppSRsv</t>
   </si>
   <si>
     <t>MailValidatorBody</t>
@@ -808,15 +799,6 @@
   </si>
   <si>
     <t>ProcessFilesFolder</t>
-  </si>
-  <si>
-    <t>D:\RUN RPA\189_HR_Workday_Casiers_Judiciaires\Prod</t>
-  </si>
-  <si>
-    <t>D:\RUN RPA\189_HR_Workday_Casiers_Judiciaires\Dev</t>
-  </si>
-  <si>
-    <t>D:\RUN RPA\189_HR_Workday_Casiers_Judiciaires\Test</t>
   </si>
   <si>
     <t>Folder where all subfolders for temporary files, such as screenshots, logfiles and statusReports are created.</t>
@@ -1235,6 +1217,48 @@
   </si>
   <si>
     <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgASr92kr_SzSLy_Z8xa3v4UAXwy55jT4JQ-YkoGyJb-1_o?e=j9aX4s</t>
+  </si>
+  <si>
+    <t>StatusRPA_NoDirection</t>
+  </si>
+  <si>
+    <t>Direction non trouvée</t>
+  </si>
+  <si>
+    <t>Data\Input</t>
+  </si>
+  <si>
+    <t>SharePointFolder_ATTENTE_RPA</t>
+  </si>
+  <si>
+    <t>Pour le dispatcher</t>
+  </si>
+  <si>
+    <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgCnlACDSukXQqIYL3FLrebzAbVMy1Sy1AptXdLHx3QJJiw?e=3H9SZl</t>
+  </si>
+  <si>
+    <t>StatusRPA_OK_Gaps</t>
+  </si>
+  <si>
+    <t>Saisie avec ecarts</t>
+  </si>
+  <si>
+    <t>SharePointFolder_FIN</t>
+  </si>
+  <si>
+    <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgArQSN-BCjMR4TUZ2wzmK5QAWkAxE-BMGG_Na9LZmex56o?e=qook5c</t>
+  </si>
+  <si>
+    <t>SENICO_DIRECTIONS</t>
+  </si>
+  <si>
+    <t>FIN;LOG;ACH;DSI</t>
+  </si>
+  <si>
+    <t>SharePointFolder_ACH</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -2133,8 +2157,8 @@
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2177,90 +2201,90 @@
         <v>6</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>7</v>
+        <v>361</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
       <c r="E4" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1">
       <c r="A5" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
       <c r="E5" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1">
       <c r="A6" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>16</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
       <c r="E6" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1">
       <c r="A7" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>19</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
       <c r="A8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>22</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1">
       <c r="A9" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>25</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
       <c r="E9" s="39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1">
@@ -2270,7 +2294,7 @@
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1">
       <c r="A11" s="88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="89"/>
       <c r="C11" s="89"/>
@@ -2279,49 +2303,49 @@
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1">
       <c r="A12" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1">
       <c r="A13" s="85" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
       <c r="E13" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1">
       <c r="A14" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>33</v>
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
       <c r="E14" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1">
       <c r="A15" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
@@ -2329,7 +2353,7 @@
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="28" t="b">
         <v>0</v>
@@ -2337,28 +2361,28 @@
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1">
       <c r="A17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>39</v>
       </c>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
       <c r="A18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>41</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>42</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
@@ -2366,10 +2390,10 @@
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1">
       <c r="A19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="28" t="s">
         <v>43</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
@@ -2377,13 +2401,13 @@
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
       <c r="A20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>46</v>
-      </c>
       <c r="C20" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="39"/>
@@ -2397,10 +2421,10 @@
     </row>
     <row r="22" spans="1:5" s="23" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="86" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
@@ -2408,10 +2432,10 @@
     </row>
     <row r="23" spans="1:5" s="23" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="86" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
@@ -2419,10 +2443,10 @@
     </row>
     <row r="24" spans="1:5" s="23" customFormat="1" ht="14.25" customHeight="1">
       <c r="A24" s="86" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
@@ -2430,7 +2454,7 @@
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1">
       <c r="A25" s="88" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="89"/>
       <c r="C25" s="89"/>
@@ -2453,7 +2477,7 @@
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="28" t="b">
         <v>1</v>
@@ -2463,12 +2487,12 @@
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="45" t="str">
         <f>IF(B9="English",LanguageSettings!$B2,IF(B9="Spanish",LanguageSettings!$D2,LanguageSettings!$C2))</f>
@@ -2477,7 +2501,7 @@
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
       <c r="E29" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1">
@@ -2488,7 +2512,7 @@
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1">
       <c r="A31" s="88" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="89"/>
       <c r="C31" s="89"/>
@@ -2497,70 +2521,70 @@
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>54</v>
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
       <c r="E32" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1">
       <c r="A33" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="30" t="s">
         <v>56</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>57</v>
       </c>
       <c r="C33" s="47"/>
       <c r="D33" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="39" t="s">
         <v>57</v>
-      </c>
-      <c r="E33" s="39" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1">
       <c r="A34" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="47"/>
       <c r="D34" s="42"/>
       <c r="E34" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1">
       <c r="A35" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="47"/>
       <c r="D35" s="42"/>
       <c r="E35" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1">
       <c r="A36" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="42"/>
       <c r="E36" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="28" t="b">
         <v>0</v>
@@ -2568,51 +2592,51 @@
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
       <c r="E37" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1">
       <c r="A38" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
       <c r="D38" s="28"/>
       <c r="E38" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1">
       <c r="A39" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>
       <c r="E39" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1">
       <c r="A40" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="C40" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="D40" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="38" t="s">
         <v>73</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1">
       <c r="A41" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" s="45">
         <v>25</v>
@@ -2620,12 +2644,12 @@
       <c r="C41" s="45"/>
       <c r="D41" s="45"/>
       <c r="E41" s="38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1">
       <c r="A42" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
@@ -2638,10 +2662,10 @@
     </row>
     <row r="44" spans="1:5" ht="15.6" customHeight="1">
       <c r="A44" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="48" t="s">
         <v>78</v>
-      </c>
-      <c r="B44" s="48" t="s">
-        <v>79</v>
       </c>
       <c r="C44" s="30"/>
       <c r="D44" s="30"/>
@@ -2649,15 +2673,15 @@
     </row>
     <row r="45" spans="1:5" ht="13.95" customHeight="1">
       <c r="A45" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="30" t="s">
         <v>80</v>
-      </c>
-      <c r="B45" s="30" t="s">
-        <v>81</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
       <c r="E45" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.95" customHeight="1">
@@ -2666,7 +2690,7 @@
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1">
       <c r="A47" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47" s="28" t="b">
         <v>1</v>
@@ -2679,27 +2703,27 @@
     </row>
     <row r="48" spans="1:5" ht="14.25" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="30" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B3,IF(B9="Spanish",LanguageSettings!$D3,LanguageSettings!$C3)),"%ProcessName%",B3)</f>
-        <v>189_HR_Workday_Casiers_Judiciaires - Status Report</v>
+        <v>SENICO - Factures fournisseurs - Status Report</v>
       </c>
       <c r="C48" s="30" t="str">
         <f>"DEV - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B3,IF(B9="Spanish",LanguageSettings!$D3,LanguageSettings!$C3)),"%ProcessName%",B3)</f>
-        <v>DEV - 189_HR_Workday_Casiers_Judiciaires - Status Report</v>
+        <v>DEV - SENICO - Factures fournisseurs - Status Report</v>
       </c>
       <c r="D48" s="30" t="str">
         <f>"INT - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B3,IF(B9="Spanish",LanguageSettings!$D3,LanguageSettings!$C3)),"%ProcessName%",B3)</f>
-        <v>INT - 189_HR_Workday_Casiers_Judiciaires - Status Report</v>
+        <v>INT - SENICO - Factures fournisseurs - Status Report</v>
       </c>
       <c r="E48" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="13.95" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B4,IF(B9="Spanish",LanguageSettings!$D4,LanguageSettings!$C4))</f>
@@ -2709,12 +2733,12 @@
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
       <c r="E49" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="14.25" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B5,IF(B9="Spanish",LanguageSettings!$D5,LanguageSettings!$C5))</f>
@@ -2723,12 +2747,12 @@
       <c r="C50" s="30"/>
       <c r="D50" s="30"/>
       <c r="E50" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13.95" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B51" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B6,IF(B9="Spanish",LanguageSettings!$D6,LanguageSettings!$C6))</f>
@@ -2737,12 +2761,12 @@
       <c r="C51" s="47"/>
       <c r="D51" s="42"/>
       <c r="E51" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.25" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B52" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B7,IF(B9="Spanish",LanguageSettings!$D7,LanguageSettings!$C7))</f>
@@ -2751,53 +2775,53 @@
       <c r="C52" s="30"/>
       <c r="D52" s="30"/>
       <c r="E52" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="14.25" customHeight="1">
       <c r="A53" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C53" s="34" t="s">
+      <c r="D53" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" s="39" t="s">
         <v>95</v>
-      </c>
-      <c r="D53" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E53" s="39" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="14.25" customHeight="1">
       <c r="A54" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="30" t="s">
         <v>97</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>98</v>
       </c>
       <c r="C54" s="30"/>
       <c r="D54" s="30"/>
       <c r="E54" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
       <c r="E55" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="14.25" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" s="30">
         <v>3</v>
@@ -2805,7 +2829,7 @@
       <c r="C56" s="30"/>
       <c r="D56" s="30"/>
       <c r="E56" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="14.25" customHeight="1">
@@ -2817,46 +2841,46 @@
     </row>
     <row r="58" spans="1:5" ht="14.25" customHeight="1">
       <c r="A58" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="30" t="s">
         <v>104</v>
-      </c>
-      <c r="B58" s="30" t="s">
-        <v>105</v>
       </c>
       <c r="C58" s="30"/>
       <c r="D58" s="30"/>
       <c r="E58" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="14.25" customHeight="1">
       <c r="A59" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="30" t="s">
         <v>107</v>
-      </c>
-      <c r="B59" s="30" t="s">
-        <v>108</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
       <c r="E59" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="14.25" customHeight="1">
       <c r="A60" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" s="30" t="s">
         <v>110</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>111</v>
       </c>
       <c r="C60" s="30"/>
       <c r="D60" s="30"/>
       <c r="E60" s="38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="14.25" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" s="28" t="b">
         <v>0</v>
@@ -2864,20 +2888,20 @@
       <c r="C61" s="30"/>
       <c r="D61" s="30"/>
       <c r="E61" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="14.25" customHeight="1">
       <c r="A62" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="28" t="s">
         <v>115</v>
-      </c>
-      <c r="B62" s="28" t="s">
-        <v>116</v>
       </c>
       <c r="C62" s="30"/>
       <c r="D62" s="30"/>
       <c r="E62" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="14.25" customHeight="1">
@@ -2889,7 +2913,7 @@
     </row>
     <row r="64" spans="1:5" ht="14.25" customHeight="1">
       <c r="A64" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64" s="28" t="b">
         <v>1</v>
@@ -2902,27 +2926,27 @@
     </row>
     <row r="65" spans="1:5" ht="14.25" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B65" s="30" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B10,IF(B9="Spanish",LanguageSettings!$D10,LanguageSettings!$C10)),"%ProcessName%",B3)</f>
-        <v>189_HR_Workday_Casiers_Judiciaires - System Exception</v>
+        <v>SENICO - Factures fournisseurs - System Exception</v>
       </c>
       <c r="C65" s="30" t="str">
         <f>"DEV - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B10,IF(B9="Spanish",LanguageSettings!$D10,LanguageSettings!$C10)),"%ProcessName%",B3)</f>
-        <v>DEV - 189_HR_Workday_Casiers_Judiciaires - System Exception</v>
+        <v>DEV - SENICO - Factures fournisseurs - System Exception</v>
       </c>
       <c r="D65" s="30" t="str">
         <f>"INT - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B10,IF(B9="Spanish",LanguageSettings!$D10,LanguageSettings!$C10)),"%ProcessName%",B3)</f>
-        <v>INT - 189_HR_Workday_Casiers_Judiciaires - System Exception</v>
+        <v>INT - SENICO - Factures fournisseurs - System Exception</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="14.25" customHeight="1">
       <c r="A66" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B66" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B11,IF(B9="Spanish",LanguageSettings!$D11,LanguageSettings!$C11))</f>
@@ -2931,12 +2955,12 @@
       <c r="C66" s="30"/>
       <c r="D66" s="30"/>
       <c r="E66" s="39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="14.25" customHeight="1">
       <c r="A67" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B67" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B12,IF(B9="Spanish",LanguageSettings!$D12,LanguageSettings!$C12))</f>
@@ -2946,48 +2970,48 @@
       <c r="C67" s="30"/>
       <c r="D67" s="30"/>
       <c r="E67" s="39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="14.25" customHeight="1">
       <c r="A68" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E68" s="39" t="s">
         <v>125</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D68" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E68" s="39" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="14.25" customHeight="1">
       <c r="A69" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C69" s="50"/>
       <c r="D69" s="50"/>
       <c r="E69" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="14.25" customHeight="1">
       <c r="A70" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B70" s="50"/>
       <c r="C70" s="50"/>
       <c r="D70" s="50"/>
       <c r="E70" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="14.25" customHeight="1">
@@ -2998,7 +3022,7 @@
     </row>
     <row r="72" spans="1:5" ht="14.25" customHeight="1">
       <c r="A72" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B72" s="28" t="b">
         <v>1</v>
@@ -3011,27 +3035,27 @@
     </row>
     <row r="73" spans="1:5" ht="14.25" customHeight="1">
       <c r="A73" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B73" s="30" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B13,IF(B9="Spanish",LanguageSettings!$D13,LanguageSettings!$C13)),"%ProcessName%",B3)</f>
-        <v>189_HR_Workday_Casiers_Judiciaires - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
+        <v>SENICO - Factures fournisseurs - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
       </c>
       <c r="C73" s="30" t="str">
         <f>"DEV - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B13,IF(B9="Spanish",LanguageSettings!$D13,LanguageSettings!$C13)),"%ProcessName%",B3)</f>
-        <v>DEV - 189_HR_Workday_Casiers_Judiciaires - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
+        <v>DEV - SENICO - Factures fournisseurs - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
       </c>
       <c r="D73" s="30" t="str">
         <f>"INT - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B13,IF(B9="Spanish",LanguageSettings!$D13,LanguageSettings!$C13)),"%ProcessName%",B3)</f>
-        <v>INT - 189_HR_Workday_Casiers_Judiciaires - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
+        <v>INT - SENICO - Factures fournisseurs - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
       </c>
       <c r="E73" s="39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="14.25" customHeight="1">
       <c r="A74" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B74" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B14,IF(B9="Spanish",LanguageSettings!$D14,LanguageSettings!$C14))</f>
@@ -3044,43 +3068,43 @@
     </row>
     <row r="75" spans="1:5" ht="14.25" customHeight="1">
       <c r="A75" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C75" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E75" s="39" t="s">
         <v>135</v>
-      </c>
-      <c r="B75" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C75" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D75" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E75" s="39" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="14.25" customHeight="1">
       <c r="A76" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" t="s">
         <v>137</v>
-      </c>
-      <c r="B76" t="s">
-        <v>138</v>
       </c>
       <c r="C76" s="28"/>
       <c r="D76" s="28"/>
       <c r="E76" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="14.25" customHeight="1">
       <c r="A77" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B77" s="28"/>
       <c r="C77" s="28"/>
       <c r="D77" s="28"/>
       <c r="E77" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="14.25" customHeight="1">
@@ -3092,7 +3116,7 @@
     </row>
     <row r="79" spans="1:5" ht="14.25" customHeight="1">
       <c r="A79" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B79" s="28" t="b">
         <v>0</v>
@@ -3102,32 +3126,32 @@
       </c>
       <c r="D79" s="28"/>
       <c r="E79" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="14.25" customHeight="1">
       <c r="A80" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B80" s="30" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B8,IF(B9="Spanish",LanguageSettings!$D8,LanguageSettings!$C8)),"%Process%",B3)</f>
-        <v>189_HR_Workday_Casiers_Judiciaires - Process Started</v>
+        <v>SENICO - Factures fournisseurs - Process Started</v>
       </c>
       <c r="C80" s="30" t="str">
         <f>"DEV - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B8,IF(B9="Spanish",LanguageSettings!$D8,LanguageSettings!$C8)),"%Process%",B3)</f>
-        <v>DEV - 189_HR_Workday_Casiers_Judiciaires - Process Started</v>
+        <v>DEV - SENICO - Factures fournisseurs - Process Started</v>
       </c>
       <c r="D80" s="30" t="str">
         <f>"INT - "&amp;SUBSTITUTE(IF(B9="English",LanguageSettings!$B8,IF(B9="Spanish",LanguageSettings!$D8,LanguageSettings!$C8)),"%Process%",B3)</f>
-        <v>INT - 189_HR_Workday_Casiers_Judiciaires - Process Started</v>
+        <v>INT - SENICO - Factures fournisseurs - Process Started</v>
       </c>
       <c r="E80" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="14.25" customHeight="1">
       <c r="A81" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B81" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B9,IF(B9="Spanish",LanguageSettings!$D9,LanguageSettings!$C9))</f>
@@ -3136,48 +3160,48 @@
       <c r="C81" s="30"/>
       <c r="D81" s="30"/>
       <c r="E81" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="14.25" customHeight="1">
       <c r="A82" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B82" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E82" s="39" t="s">
         <v>148</v>
-      </c>
-      <c r="B82" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C82" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D82" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E82" s="39" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="14.25" customHeight="1">
       <c r="A83" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C83" s="28"/>
       <c r="D83" s="28"/>
       <c r="E83" s="39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="14.25" customHeight="1">
       <c r="A84" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B84" s="30"/>
       <c r="C84" s="28"/>
       <c r="D84" s="28"/>
       <c r="E84" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -3240,11 +3264,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3276,7 +3300,7 @@
     </row>
     <row r="2" spans="1:14" s="60" customFormat="1" ht="15.6" customHeight="1">
       <c r="A2" s="57" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B2" s="58"/>
       <c r="C2" s="58"/>
@@ -3285,15 +3309,15 @@
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1">
       <c r="A3" s="61" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>154</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>155</v>
       </c>
       <c r="C3" s="63"/>
       <c r="D3" s="63"/>
       <c r="E3" s="64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F3" s="63"/>
       <c r="G3" s="63"/>
@@ -3307,15 +3331,15 @@
     </row>
     <row r="4" spans="1:14" ht="14.25" customHeight="1">
       <c r="A4" s="61" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="62" t="s">
         <v>157</v>
-      </c>
-      <c r="B4" s="62" t="s">
-        <v>158</v>
       </c>
       <c r="C4" s="63"/>
       <c r="D4" s="63"/>
       <c r="E4" s="64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F4" s="63"/>
       <c r="G4" s="63"/>
@@ -3329,15 +3353,15 @@
     </row>
     <row r="5" spans="1:14" ht="14.25" customHeight="1">
       <c r="A5" s="61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="63"/>
       <c r="D5" s="63"/>
       <c r="E5" s="64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F5" s="63"/>
       <c r="G5" s="63"/>
@@ -3351,7 +3375,7 @@
     </row>
     <row r="6" spans="1:14" s="70" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="66" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -3360,17 +3384,17 @@
     </row>
     <row r="7" spans="1:14" ht="14.25" customHeight="1">
       <c r="A7" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="62" t="s">
         <v>160</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>161</v>
       </c>
       <c r="C7" s="63"/>
       <c r="D7" s="63"/>
     </row>
     <row r="8" spans="1:14" ht="14.25" customHeight="1">
       <c r="A8" s="71" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="62">
         <v>20</v>
@@ -3380,101 +3404,101 @@
     </row>
     <row r="9" spans="1:14" ht="14.25" customHeight="1">
       <c r="A9" s="71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C9" s="63"/>
       <c r="D9" s="63"/>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1">
       <c r="A10" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>165</v>
-      </c>
       <c r="C10" s="63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D10" s="63"/>
     </row>
     <row r="11" spans="1:14" ht="14.25" customHeight="1">
       <c r="A11" s="71" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>167</v>
-      </c>
       <c r="C11" s="63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D11" s="63"/>
     </row>
     <row r="12" spans="1:14" ht="14.25" customHeight="1">
       <c r="A12" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>169</v>
-      </c>
       <c r="C12" s="63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" s="63"/>
     </row>
     <row r="13" spans="1:14" ht="14.25" customHeight="1">
       <c r="A13" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="62" t="s">
-        <v>171</v>
-      </c>
       <c r="C13" s="63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D13" s="63"/>
     </row>
     <row r="14" spans="1:14" ht="14.25" customHeight="1">
       <c r="A14" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="73" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="73" t="s">
-        <v>173</v>
-      </c>
       <c r="C14" s="65" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14" s="63"/>
     </row>
     <row r="15" spans="1:14" ht="14.25" customHeight="1">
       <c r="A15" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="B15" s="73" t="s">
-        <v>175</v>
-      </c>
       <c r="C15" s="65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D15" s="63"/>
     </row>
     <row r="16" spans="1:14" ht="14.25" customHeight="1">
       <c r="A16" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="73" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="73" t="s">
-        <v>177</v>
-      </c>
       <c r="C16" s="65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D16" s="63"/>
     </row>
     <row r="17" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="66" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B17" s="67"/>
       <c r="C17" s="68"/>
@@ -3483,79 +3507,79 @@
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
       <c r="A18" s="71" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="73" t="s">
         <v>178</v>
-      </c>
-      <c r="B18" s="73" t="s">
-        <v>179</v>
       </c>
       <c r="C18" s="65"/>
       <c r="D18" s="63"/>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1">
       <c r="A19" s="71" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" s="73" t="s">
         <v>180</v>
-      </c>
-      <c r="B19" s="73" t="s">
-        <v>181</v>
       </c>
       <c r="C19" s="65"/>
       <c r="D19" s="63"/>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
       <c r="A20" s="71" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B20" s="73" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C20" s="65"/>
       <c r="D20" s="63"/>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1">
       <c r="A21" s="71" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B21" s="73" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="63"/>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1">
       <c r="A22" s="71" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B22" s="73" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C22" s="65"/>
       <c r="D22" s="63"/>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
       <c r="A23" s="71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C23" s="65"/>
       <c r="D23" s="63"/>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1">
       <c r="A24" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="B24" s="73" t="s">
-        <v>184</v>
-      </c>
       <c r="C24" s="65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D24" s="63"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1">
       <c r="A25" s="71" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B25" s="73">
         <v>0.5</v>
@@ -3567,306 +3591,313 @@
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1">
       <c r="A26" s="71" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D26" s="63"/>
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1">
       <c r="A27" s="71" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C27" s="65" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D27" s="63"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="71" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B28" s="75" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C28" s="76" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D28" s="63"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="71" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B29" s="73" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C29" s="65" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D29" s="63"/>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1">
       <c r="A30" s="71" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B30" s="73" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D30" s="63"/>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1">
       <c r="A31" s="84" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B31" s="83" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="63"/>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1">
       <c r="A32" s="84" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B32" s="83" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="63"/>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1">
       <c r="A33" s="84" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="B33" s="83" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C33" s="65"/>
       <c r="D33" s="63"/>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1">
       <c r="A34" s="84" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B34" s="83" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C34" s="65"/>
       <c r="D34" s="63"/>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A35" s="71"/>
-      <c r="B35" s="73"/>
+      <c r="A35" s="84" t="s">
+        <v>384</v>
+      </c>
+      <c r="B35" s="73" t="s">
+        <v>385</v>
+      </c>
       <c r="C35" s="65"/>
       <c r="D35" s="63"/>
     </row>
-    <row r="36" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="66" t="s">
-        <v>371</v>
-      </c>
-      <c r="B36" s="67"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="69"/>
-    </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A37" s="71" t="s">
-        <v>359</v>
-      </c>
-      <c r="B37" s="73" t="s">
-        <v>360</v>
-      </c>
-      <c r="C37" s="65" t="s">
-        <v>186</v>
-      </c>
-      <c r="D37" s="63"/>
+    <row r="36" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A36" s="84" t="s">
+        <v>390</v>
+      </c>
+      <c r="B36" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="C36" s="65"/>
+      <c r="D36" s="63"/>
+    </row>
+    <row r="37" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A37" s="66" t="s">
+        <v>365</v>
+      </c>
+      <c r="B37" s="67"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="69"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1">
       <c r="A38" s="71" t="s">
-        <v>388</v>
+        <v>353</v>
       </c>
       <c r="B38" s="73" t="s">
-        <v>389</v>
-      </c>
-      <c r="C38" s="65"/>
+        <v>354</v>
+      </c>
+      <c r="C38" s="65" t="s">
+        <v>185</v>
+      </c>
       <c r="D38" s="63"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1">
       <c r="A39" s="71" t="s">
-        <v>361</v>
+        <v>382</v>
       </c>
       <c r="B39" s="73" t="s">
-        <v>362</v>
+        <v>383</v>
       </c>
       <c r="C39" s="65"/>
       <c r="D39" s="63"/>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1">
       <c r="A40" s="71" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B40" s="73" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C40" s="65"/>
       <c r="D40" s="63"/>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1">
       <c r="A41" s="71" t="s">
-        <v>193</v>
+        <v>357</v>
       </c>
       <c r="B41" s="73" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="63"/>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1">
       <c r="A42" s="71" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B42" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="C42" s="65" t="s">
-        <v>188</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="C42" s="65"/>
       <c r="D42" s="63"/>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1">
       <c r="A43" s="71" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B43" s="73" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C43" s="65" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D43" s="63"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" customHeight="1">
       <c r="A44" s="71" t="s">
-        <v>191</v>
+        <v>396</v>
       </c>
       <c r="B44" s="73" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D44" s="63"/>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1">
       <c r="A45" s="71" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B45" s="73" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D45" s="63"/>
     </row>
-    <row r="46" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="66" t="s">
-        <v>373</v>
-      </c>
-      <c r="B46" s="67"/>
-      <c r="C46" s="68"/>
-      <c r="D46" s="68"/>
-      <c r="E46" s="69"/>
-    </row>
-    <row r="47" spans="1:5" ht="13.2" customHeight="1">
+    <row r="46" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A46" s="71" t="s">
+        <v>392</v>
+      </c>
+      <c r="B46" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="C46" s="65"/>
+      <c r="D46" s="63"/>
+    </row>
+    <row r="47" spans="1:5" ht="14.25" customHeight="1">
       <c r="A47" s="71" t="s">
-        <v>343</v>
-      </c>
-      <c r="B47" s="77" t="s">
+        <v>387</v>
+      </c>
+      <c r="B47" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="C47" s="65"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="72" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A48" s="66" t="s">
+        <v>367</v>
+      </c>
+      <c r="B48" s="67"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="69"/>
+    </row>
+    <row r="49" spans="1:5" ht="13.2" customHeight="1">
+      <c r="A49" s="71" t="s">
+        <v>337</v>
+      </c>
+      <c r="B49" s="77" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="13.2" customHeight="1">
+      <c r="A50" s="79" t="s">
+        <v>338</v>
+      </c>
+      <c r="B50" s="80" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="13.2" customHeight="1">
-      <c r="A48" s="79" t="s">
-        <v>344</v>
-      </c>
-      <c r="B48" s="80" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="13.2" customHeight="1">
-      <c r="A49" s="79" t="s">
-        <v>345</v>
-      </c>
-      <c r="B49" s="80" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1">
-      <c r="A50" s="71" t="s">
-        <v>320</v>
-      </c>
-      <c r="B50" s="62" t="s">
-        <v>329</v>
-      </c>
-      <c r="D50" s="63"/>
-      <c r="E50" s="72" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1">
-      <c r="A51" s="71" t="s">
-        <v>331</v>
-      </c>
-      <c r="B51" s="73" t="s">
-        <v>337</v>
-      </c>
-      <c r="D51" s="63"/>
+    <row r="51" spans="1:5" ht="13.2" customHeight="1">
+      <c r="A51" s="79" t="s">
+        <v>339</v>
+      </c>
+      <c r="B51" s="80" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1">
       <c r="A52" s="71" t="s">
-        <v>332</v>
-      </c>
-      <c r="B52" s="73" t="s">
-        <v>338</v>
+        <v>314</v>
+      </c>
+      <c r="B52" s="62" t="s">
+        <v>323</v>
       </c>
       <c r="D52" s="63"/>
+      <c r="E52" s="72" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1">
       <c r="A53" s="71" t="s">
-        <v>330</v>
-      </c>
-      <c r="B53" s="62" t="s">
-        <v>321</v>
+        <v>325</v>
+      </c>
+      <c r="B53" s="73" t="s">
+        <v>331</v>
       </c>
       <c r="D53" s="63"/>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1">
       <c r="A54" s="71" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B54" s="73" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D54" s="63"/>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1">
       <c r="A55" s="71" t="s">
-        <v>334</v>
-      </c>
-      <c r="B55" s="73" t="s">
-        <v>342</v>
+        <v>324</v>
+      </c>
+      <c r="B55" s="62" t="s">
+        <v>315</v>
       </c>
       <c r="D55" s="63"/>
     </row>
@@ -3874,91 +3905,104 @@
       <c r="A56" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="B56" s="62" t="s">
-        <v>328</v>
+      <c r="B56" s="73" t="s">
+        <v>335</v>
       </c>
       <c r="D56" s="63"/>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1">
       <c r="A57" s="71" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B57" s="73" t="s">
-        <v>339</v>
-      </c>
-      <c r="C57" s="62"/>
+        <v>336</v>
+      </c>
       <c r="D57" s="63"/>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1">
       <c r="A58" s="71" t="s">
-        <v>336</v>
-      </c>
-      <c r="B58" s="73" t="s">
-        <v>340</v>
-      </c>
-      <c r="C58" s="62"/>
+        <v>321</v>
+      </c>
+      <c r="B58" s="62" t="s">
+        <v>322</v>
+      </c>
       <c r="D58" s="63"/>
     </row>
-    <row r="59" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A59" s="66" t="s">
-        <v>372</v>
-      </c>
-      <c r="B59" s="67"/>
-      <c r="C59" s="68"/>
-      <c r="D59" s="68"/>
-      <c r="E59" s="69"/>
-    </row>
-    <row r="60" spans="1:5" ht="28.8">
+    <row r="59" spans="1:5" ht="15" customHeight="1">
+      <c r="A59" s="71" t="s">
+        <v>329</v>
+      </c>
+      <c r="B59" s="73" t="s">
+        <v>333</v>
+      </c>
+      <c r="C59" s="62"/>
+      <c r="D59" s="63"/>
+    </row>
+    <row r="60" spans="1:5" ht="15" customHeight="1">
       <c r="A60" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="B60" s="62" t="s">
-        <v>325</v>
-      </c>
-      <c r="C60" s="63"/>
+        <v>330</v>
+      </c>
+      <c r="B60" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="C60" s="62"/>
       <c r="D60" s="63"/>
     </row>
-    <row r="61" spans="1:5" ht="72">
-      <c r="A61" s="71" t="s">
-        <v>324</v>
-      </c>
-      <c r="B61" s="62" t="s">
-        <v>326</v>
-      </c>
-      <c r="C61" s="63"/>
-      <c r="D61" s="63"/>
-    </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1">
-      <c r="A62" s="71"/>
-      <c r="B62" s="62"/>
+    <row r="61" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A61" s="66" t="s">
+        <v>366</v>
+      </c>
+      <c r="B61" s="67"/>
+      <c r="C61" s="68"/>
+      <c r="D61" s="68"/>
+      <c r="E61" s="69"/>
+    </row>
+    <row r="62" spans="1:5" ht="28.8">
+      <c r="A62" s="71" t="s">
+        <v>317</v>
+      </c>
+      <c r="B62" s="62" t="s">
+        <v>319</v>
+      </c>
       <c r="C62" s="63"/>
       <c r="D62" s="63"/>
     </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1">
-      <c r="A63" s="81" t="s">
-        <v>348</v>
-      </c>
-      <c r="B63" s="77" t="s">
-        <v>349</v>
+    <row r="63" spans="1:5" ht="72">
+      <c r="A63" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="B63" s="62" t="s">
+        <v>320</v>
       </c>
       <c r="C63" s="63"/>
       <c r="D63" s="63"/>
     </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1">
-      <c r="A64" s="71"/>
-      <c r="B64" s="62"/>
-      <c r="C64" s="63"/>
-      <c r="D64" s="63"/>
+    <row r="64" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A64" s="66" t="s">
+        <v>397</v>
+      </c>
+      <c r="B64" s="67"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="69"/>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1">
-      <c r="A65" s="71"/>
-      <c r="B65" s="62"/>
+      <c r="A65" s="81" t="s">
+        <v>342</v>
+      </c>
+      <c r="B65" s="77" t="s">
+        <v>343</v>
+      </c>
       <c r="C65" s="63"/>
       <c r="D65" s="63"/>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1">
-      <c r="A66" s="71"/>
-      <c r="B66" s="62"/>
+      <c r="A66" s="71" t="s">
+        <v>394</v>
+      </c>
+      <c r="B66" s="62" t="s">
+        <v>395</v>
+      </c>
       <c r="C66" s="63"/>
       <c r="D66" s="63"/>
     </row>
@@ -4111,6 +4155,18 @@
       <c r="B91" s="62"/>
       <c r="C91" s="63"/>
       <c r="D91" s="63"/>
+    </row>
+    <row r="92" spans="1:4" ht="15" customHeight="1">
+      <c r="A92" s="71"/>
+      <c r="B92" s="62"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="63"/>
+    </row>
+    <row r="93" spans="1:4" ht="15" customHeight="1">
+      <c r="A93" s="71"/>
+      <c r="B93" s="62"/>
+      <c r="C93" s="63"/>
+      <c r="D93" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4127,14 +4183,14 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.21875" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" customWidth="1"/>
     <col min="4" max="4" width="14.21875" customWidth="1"/>
     <col min="5" max="5" width="143.44140625" customWidth="1"/>
@@ -4159,7 +4215,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="91" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B2" s="92"/>
       <c r="C2" s="92"/>
@@ -4168,7 +4224,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B3" s="19">
         <v>0</v>
@@ -4176,12 +4232,12 @@
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="20" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B4" s="3">
         <v>200</v>
@@ -4189,12 +4245,12 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -4202,12 +4258,12 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1">
       <c r="A6" s="14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B6" s="15">
         <v>3</v>
@@ -4215,13 +4271,13 @@
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B8" s="19">
         <v>5</v>
@@ -4229,12 +4285,12 @@
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="20" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1">
       <c r="A9" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B9" s="3">
         <v>30</v>
@@ -4242,12 +4298,12 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1">
       <c r="A10" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B10" s="15">
         <v>120</v>
@@ -4255,13 +4311,13 @@
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:5" ht="14.25" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B12" s="19">
         <v>1</v>
@@ -4269,12 +4325,12 @@
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B13" s="3">
         <v>15</v>
@@ -4282,12 +4338,12 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="12" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B14" s="15">
         <v>60</v>
@@ -4295,13 +4351,13 @@
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="16" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:5" ht="14.25" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B16" s="19">
         <v>0.6</v>
@@ -4309,12 +4365,12 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1">
       <c r="A17" s="13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B17" s="3">
         <v>0.8</v>
@@ -4322,12 +4378,12 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B18" s="15">
         <v>0.9</v>
@@ -4335,92 +4391,92 @@
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1">
       <c r="A21" s="13" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1">
       <c r="A22" s="13" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
       <c r="A23" s="13" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="16" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:5" ht="14.25" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B27" s="19">
         <v>0</v>
@@ -4428,12 +4484,12 @@
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
       <c r="E27" s="20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="13" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -4441,12 +4497,12 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B29" s="15">
         <v>0</v>
@@ -4454,30 +4510,26 @@
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="16" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:5" ht="14.25" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>256</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="20" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.1" customHeight="1">
       <c r="A32" s="14" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B32" s="15">
         <v>7</v>
@@ -4485,13 +4537,13 @@
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="16" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.1" customHeight="1"/>
     <row r="34" spans="1:5" ht="14.1" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B34" s="19">
         <v>3</v>
@@ -4499,12 +4551,12 @@
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="20" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.1" customHeight="1">
       <c r="A35" s="14" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B35" s="15">
         <v>5</v>
@@ -4512,13 +4564,13 @@
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="16" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:5" ht="14.25" customHeight="1">
       <c r="A37" s="94" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B37" s="95"/>
       <c r="C37" s="95"/>
@@ -4527,7 +4579,7 @@
     </row>
     <row r="38" spans="1:5" s="17" customFormat="1" ht="14.25" customHeight="1">
       <c r="A38" s="21" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -4569,21 +4621,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4591,10 +4643,10 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4649,220 +4701,220 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4">
       <c r="A3" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="89.25" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="89.25" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="89.25" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="89.25" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.4">
       <c r="A8" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="89.25" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="14.4">
       <c r="A10" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="89.25" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="178.95" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2">
       <c r="A13" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="134.55000000000001" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="134.55000000000001" customHeight="1">
@@ -4897,57 +4949,57 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suppression du globalHandler. E2E gestion des nouvelles transactions. Reste le CR
</commit_message>
<xml_diff>
--- a/Configuration/Config_AR.xlsx
+++ b/Configuration/Config_AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Travail\SynologyDrive\Pro\Projets Pro\UiPath RPA\Studio\0. SENICO\rpa-senico-factures-frs\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\Dev\Clients\SENICO\rpa-senico-factures-frs\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C50F7FD-6B82-46C7-96AC-6D4F11DBBE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E0428-7F10-489B-A704-848E655D107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="23016" windowHeight="14460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="400">
   <si>
     <t>Name</t>
   </si>
@@ -1259,6 +1259,12 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>StatusRPA_KO_Other</t>
+  </si>
+  <si>
+    <t>Autre erreur</t>
   </si>
 </sst>
 </file>
@@ -3264,11 +3270,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N93"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3701,390 +3707,394 @@
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1">
       <c r="A36" s="84" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="B36" s="73" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="C36" s="65"/>
       <c r="D36" s="63"/>
     </row>
-    <row r="37" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A37" s="66" t="s">
+    <row r="37" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A37" s="84" t="s">
+        <v>390</v>
+      </c>
+      <c r="B37" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="C37" s="65"/>
+      <c r="D37" s="63"/>
+    </row>
+    <row r="38" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A38" s="66" t="s">
         <v>365</v>
       </c>
-      <c r="B37" s="67"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="69"/>
-    </row>
-    <row r="38" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A38" s="71" t="s">
-        <v>353</v>
-      </c>
-      <c r="B38" s="73" t="s">
-        <v>354</v>
-      </c>
-      <c r="C38" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="D38" s="63"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1">
       <c r="A39" s="71" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="B39" s="73" t="s">
-        <v>383</v>
-      </c>
-      <c r="C39" s="65"/>
+        <v>354</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>185</v>
+      </c>
       <c r="D39" s="63"/>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1">
       <c r="A40" s="71" t="s">
-        <v>355</v>
+        <v>382</v>
       </c>
       <c r="B40" s="73" t="s">
-        <v>356</v>
+        <v>383</v>
       </c>
       <c r="C40" s="65"/>
       <c r="D40" s="63"/>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1">
       <c r="A41" s="71" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B41" s="73" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="63"/>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1">
       <c r="A42" s="71" t="s">
-        <v>191</v>
+        <v>357</v>
       </c>
       <c r="B42" s="73" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C42" s="65"/>
       <c r="D42" s="63"/>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1">
       <c r="A43" s="71" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B43" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="C43" s="65" t="s">
-        <v>187</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="C43" s="65"/>
       <c r="D43" s="63"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" customHeight="1">
       <c r="A44" s="71" t="s">
-        <v>396</v>
+        <v>186</v>
       </c>
       <c r="B44" s="73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D44" s="63"/>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1">
       <c r="A45" s="71" t="s">
-        <v>189</v>
+        <v>396</v>
       </c>
       <c r="B45" s="73" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D45" s="63"/>
     </row>
     <row r="46" spans="1:5" ht="14.25" customHeight="1">
       <c r="A46" s="71" t="s">
-        <v>392</v>
+        <v>189</v>
       </c>
       <c r="B46" s="73" t="s">
-        <v>393</v>
-      </c>
-      <c r="C46" s="65"/>
+        <v>190</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>190</v>
+      </c>
       <c r="D46" s="63"/>
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1">
       <c r="A47" s="71" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="B47" s="73" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C47" s="65"/>
       <c r="D47" s="63"/>
-      <c r="E47" s="72" t="s">
+    </row>
+    <row r="48" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A48" s="71" t="s">
+        <v>387</v>
+      </c>
+      <c r="B48" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="C48" s="65"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="72" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="66" t="s">
+    <row r="49" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A49" s="66" t="s">
         <v>367</v>
       </c>
-      <c r="B48" s="67"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="69"/>
-    </row>
-    <row r="49" spans="1:5" ht="13.2" customHeight="1">
-      <c r="A49" s="71" t="s">
+      <c r="B49" s="67"/>
+      <c r="C49" s="68"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="69"/>
+    </row>
+    <row r="50" spans="1:5" ht="13.2" customHeight="1">
+      <c r="A50" s="71" t="s">
         <v>337</v>
       </c>
-      <c r="B49" s="77" t="s">
+      <c r="B50" s="77" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="13.2" customHeight="1">
-      <c r="A50" s="79" t="s">
-        <v>338</v>
-      </c>
-      <c r="B50" s="80" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13.2" customHeight="1">
       <c r="A51" s="79" t="s">
+        <v>338</v>
+      </c>
+      <c r="B51" s="80" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="13.2" customHeight="1">
+      <c r="A52" s="79" t="s">
         <v>339</v>
       </c>
-      <c r="B51" s="80" t="s">
+      <c r="B52" s="80" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1">
-      <c r="A52" s="71" t="s">
-        <v>314</v>
-      </c>
-      <c r="B52" s="62" t="s">
-        <v>323</v>
-      </c>
-      <c r="D52" s="63"/>
-      <c r="E52" s="72" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1">
       <c r="A53" s="71" t="s">
-        <v>325</v>
-      </c>
-      <c r="B53" s="73" t="s">
-        <v>331</v>
+        <v>314</v>
+      </c>
+      <c r="B53" s="62" t="s">
+        <v>323</v>
       </c>
       <c r="D53" s="63"/>
+      <c r="E53" s="72" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1">
       <c r="A54" s="71" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B54" s="73" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D54" s="63"/>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1">
       <c r="A55" s="71" t="s">
-        <v>324</v>
-      </c>
-      <c r="B55" s="62" t="s">
-        <v>315</v>
+        <v>326</v>
+      </c>
+      <c r="B55" s="73" t="s">
+        <v>332</v>
       </c>
       <c r="D55" s="63"/>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1">
       <c r="A56" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B56" s="73" t="s">
-        <v>335</v>
+        <v>324</v>
+      </c>
+      <c r="B56" s="62" t="s">
+        <v>315</v>
       </c>
       <c r="D56" s="63"/>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1">
       <c r="A57" s="71" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B57" s="73" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D57" s="63"/>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1">
       <c r="A58" s="71" t="s">
-        <v>321</v>
-      </c>
-      <c r="B58" s="62" t="s">
-        <v>322</v>
+        <v>328</v>
+      </c>
+      <c r="B58" s="73" t="s">
+        <v>336</v>
       </c>
       <c r="D58" s="63"/>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1">
       <c r="A59" s="71" t="s">
-        <v>329</v>
-      </c>
-      <c r="B59" s="73" t="s">
-        <v>333</v>
-      </c>
-      <c r="C59" s="62"/>
+        <v>321</v>
+      </c>
+      <c r="B59" s="62" t="s">
+        <v>322</v>
+      </c>
       <c r="D59" s="63"/>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1">
       <c r="A60" s="71" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B60" s="73" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C60" s="62"/>
       <c r="D60" s="63"/>
     </row>
-    <row r="61" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A61" s="66" t="s">
+    <row r="61" spans="1:5" ht="15" customHeight="1">
+      <c r="A61" s="71" t="s">
+        <v>330</v>
+      </c>
+      <c r="B61" s="73" t="s">
+        <v>334</v>
+      </c>
+      <c r="C61" s="62"/>
+      <c r="D61" s="63"/>
+    </row>
+    <row r="62" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A62" s="66" t="s">
         <v>366</v>
       </c>
-      <c r="B61" s="67"/>
-      <c r="C61" s="68"/>
-      <c r="D61" s="68"/>
-      <c r="E61" s="69"/>
-    </row>
-    <row r="62" spans="1:5" ht="28.8">
-      <c r="A62" s="71" t="s">
+      <c r="B62" s="67"/>
+      <c r="C62" s="68"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="69"/>
+    </row>
+    <row r="63" spans="1:5" ht="28.8">
+      <c r="A63" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B62" s="62" t="s">
+      <c r="B63" s="62" t="s">
         <v>319</v>
-      </c>
-      <c r="C62" s="63"/>
-      <c r="D62" s="63"/>
-    </row>
-    <row r="63" spans="1:5" ht="72">
-      <c r="A63" s="71" t="s">
-        <v>318</v>
-      </c>
-      <c r="B63" s="62" t="s">
-        <v>320</v>
       </c>
       <c r="C63" s="63"/>
       <c r="D63" s="63"/>
     </row>
-    <row r="64" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A64" s="66" t="s">
+    <row r="64" spans="1:5" ht="72">
+      <c r="A64" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="B64" s="62" t="s">
+        <v>320</v>
+      </c>
+      <c r="C64" s="63"/>
+      <c r="D64" s="63"/>
+    </row>
+    <row r="65" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A65" s="66" t="s">
         <v>397</v>
       </c>
-      <c r="B64" s="67"/>
-      <c r="C64" s="68"/>
-      <c r="D64" s="68"/>
-      <c r="E64" s="69"/>
-    </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1">
-      <c r="A65" s="81" t="s">
+      <c r="B65" s="67"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="69"/>
+    </row>
+    <row r="66" spans="1:5" ht="15" customHeight="1">
+      <c r="A66" s="81" t="s">
         <v>342</v>
       </c>
-      <c r="B65" s="77" t="s">
+      <c r="B66" s="77" t="s">
         <v>343</v>
-      </c>
-      <c r="C65" s="63"/>
-      <c r="D65" s="63"/>
-    </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1">
-      <c r="A66" s="71" t="s">
-        <v>394</v>
-      </c>
-      <c r="B66" s="62" t="s">
-        <v>395</v>
       </c>
       <c r="C66" s="63"/>
       <c r="D66" s="63"/>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1">
-      <c r="A67" s="71"/>
-      <c r="B67" s="62"/>
+    <row r="67" spans="1:5" ht="15" customHeight="1">
+      <c r="A67" s="71" t="s">
+        <v>394</v>
+      </c>
+      <c r="B67" s="62" t="s">
+        <v>395</v>
+      </c>
       <c r="C67" s="63"/>
       <c r="D67" s="63"/>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1">
+    <row r="68" spans="1:5" ht="15" customHeight="1">
       <c r="A68" s="71"/>
       <c r="B68" s="62"/>
       <c r="C68" s="63"/>
       <c r="D68" s="63"/>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1">
+    <row r="69" spans="1:5" ht="15" customHeight="1">
       <c r="A69" s="71"/>
       <c r="B69" s="62"/>
       <c r="C69" s="63"/>
       <c r="D69" s="63"/>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1">
+    <row r="70" spans="1:5" ht="15" customHeight="1">
       <c r="A70" s="71"/>
       <c r="B70" s="62"/>
       <c r="C70" s="63"/>
       <c r="D70" s="63"/>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1">
+    <row r="71" spans="1:5" ht="15" customHeight="1">
       <c r="A71" s="71"/>
       <c r="B71" s="62"/>
       <c r="C71" s="63"/>
       <c r="D71" s="63"/>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1">
+    <row r="72" spans="1:5" ht="15" customHeight="1">
       <c r="A72" s="71"/>
       <c r="B72" s="62"/>
       <c r="C72" s="63"/>
       <c r="D72" s="63"/>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1">
+    <row r="73" spans="1:5" ht="15" customHeight="1">
       <c r="A73" s="71"/>
       <c r="B73" s="62"/>
       <c r="C73" s="63"/>
       <c r="D73" s="63"/>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1">
+    <row r="74" spans="1:5" ht="15" customHeight="1">
       <c r="A74" s="71"/>
       <c r="B74" s="62"/>
       <c r="C74" s="63"/>
       <c r="D74" s="63"/>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1">
+    <row r="75" spans="1:5" ht="15" customHeight="1">
       <c r="A75" s="71"/>
       <c r="B75" s="62"/>
       <c r="C75" s="63"/>
       <c r="D75" s="63"/>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1">
+    <row r="76" spans="1:5" ht="15" customHeight="1">
       <c r="A76" s="71"/>
       <c r="B76" s="62"/>
       <c r="C76" s="63"/>
       <c r="D76" s="63"/>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1">
+    <row r="77" spans="1:5" ht="15" customHeight="1">
       <c r="A77" s="71"/>
       <c r="B77" s="62"/>
       <c r="C77" s="63"/>
       <c r="D77" s="63"/>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1">
+    <row r="78" spans="1:5" ht="15" customHeight="1">
       <c r="A78" s="71"/>
       <c r="B78" s="62"/>
       <c r="C78" s="63"/>
       <c r="D78" s="63"/>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1">
+    <row r="79" spans="1:5" ht="15" customHeight="1">
       <c r="A79" s="71"/>
       <c r="B79" s="62"/>
       <c r="C79" s="63"/>
       <c r="D79" s="63"/>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1">
+    <row r="80" spans="1:5" ht="15" customHeight="1">
       <c r="A80" s="71"/>
       <c r="B80" s="62"/>
       <c r="C80" s="63"/>
@@ -4167,6 +4177,12 @@
       <c r="B93" s="62"/>
       <c r="C93" s="63"/>
       <c r="D93" s="63"/>
+    </row>
+    <row r="94" spans="1:4" ht="15" customHeight="1">
+      <c r="A94" s="71"/>
+      <c r="B94" s="62"/>
+      <c r="C94" s="63"/>
+      <c r="D94" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add CR HTML Email send
</commit_message>
<xml_diff>
--- a/Configuration/Config_AR.xlsx
+++ b/Configuration/Config_AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\Dev\Clients\SENICO\rpa-senico-factures-frs\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\senyone\rpa-senico-factures-frs\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E0428-7F10-489B-A704-848E655D107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C085CAB9-1966-401D-8BE0-0AC870146A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="417">
   <si>
     <t>Name</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>ProcessesToKill</t>
-  </si>
-  <si>
-    <t>chrome</t>
   </si>
   <si>
     <t>String containing the names of the processes to be killed in the KillAllProcesses workflow. Default Delimiter " ; ". Example: iexplore;chrome; …</t>
@@ -1147,9 +1144,6 @@
     <t>https://senyone.sharepoint.com/:f:/s/ServicesRH/IgAbdU_t7HW4So2YznO6G_5wAUB7d_upIMseXAUSlG6b6oo?e=axNNT3</t>
   </si>
   <si>
-    <t>bilal@senyone.sn's workspace</t>
-  </si>
-  <si>
     <t>SENICO - Factures fournisseurs</t>
   </si>
   <si>
@@ -1265,6 +1259,63 @@
   </si>
   <si>
     <t>Autre erreur</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>orlando.bita@senyone.sn's workspace</t>
+  </si>
+  <si>
+    <t>SendMailForCR</t>
+  </si>
+  <si>
+    <t>CR_Mail_Subject</t>
+  </si>
+  <si>
+    <t>CR_Mail_CustomMessage</t>
+  </si>
+  <si>
+    <t>CR_Mail_Receiver</t>
+  </si>
+  <si>
+    <t>CR_Mail_ReceiverCC</t>
+  </si>
+  <si>
+    <t>CR_Mail_ReceiverBCC</t>
+  </si>
+  <si>
+    <t>orlando.bita@senyone.sn</t>
+  </si>
+  <si>
+    <t>SENICO - Factures Fournisseurs - Compte Rendu</t>
+  </si>
+  <si>
+    <t>CR_Mail_ErrorDetails</t>
+  </si>
+  <si>
+    <t>Subject of CR Mail which is sent at the end of the process if SendMailForCR is set to True</t>
+  </si>
+  <si>
+    <t>CR Message body template. See Also Sheet LanguageSettings</t>
+  </si>
+  <si>
+    <t>CR Message part which contain Error Details. See Also Sheet LanguageSettings</t>
+  </si>
+  <si>
+    <t>Receiver of CR Mail. Seperate multiple mailaddresses with a ; symbol, e.g. 123@roboyo.de; 456@roboyo.de</t>
+  </si>
+  <si>
+    <t>Receiver of CR Mail in CC. Seperate multiple mailaddresses with a ; symbol, e.g. 123@roboyo.de; 456@roboyo.de</t>
+  </si>
+  <si>
+    <t>Receiver of CR Mail in BCC. Seperate multiple mailaddresses with a ; symbol, e.g. 123@roboyo.de; 456@roboyo.de</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Détails des erreurs :&lt;/strong&gt;&lt;/p&gt;&lt;table border="1" cellpadding="0" cellspacing="0" width="750" style="width: 750px; table-layout: fixed; border-collapse: collapse;"&gt;&lt;thead&gt;&lt;tr&gt;&lt;th style="width: 250px;"&gt;Nom Fichier&lt;/th&gt;&lt;th style="width: 250px;"&gt;URL SharePoint&lt;/th&gt;&lt;th style="width: 250px;"&gt;Message d'erreur&lt;/th&gt;&lt;/tr&gt;&lt;/thead&gt;&lt;tbody&gt;%ErrorDetailRow%&lt;/tbody&gt;&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ci-dessous le rapport d'exécution du process du {0} :&lt;br/&gt;# Nombre de mails lus : {1}&lt;br/&gt;# Nombre de fichiers traités : {2}&lt;br/&gt;# Nombre de traitements réussis : {3}&lt;br/&gt;# Nombre de traitements échoués : {4}&lt;br/&gt;# Nombre de traitements avec écarts : {5}&lt;br&gt;%ErrorsDetails%&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1664,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1869,10 +1920,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="40 % - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2160,20 +2214,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="50.5546875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="49.77734375" style="25" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="130.21875" style="37" customWidth="1"/>
+    <col min="1" max="1" width="50.5234375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="49.7890625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="28.68359375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="28.41796875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="130.20703125" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="22" customFormat="1" ht="15.6" customHeight="1">
@@ -2207,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -2220,7 +2274,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -2272,25 +2326,25 @@
         <v>20</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>21</v>
+        <v>398</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1">
       <c r="A9" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>24</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
       <c r="E9" s="39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1">
@@ -2300,7 +2354,7 @@
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1">
       <c r="A11" s="88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="89"/>
       <c r="C11" s="89"/>
@@ -2309,49 +2363,49 @@
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1">
       <c r="A12" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1">
       <c r="A13" s="85" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>360</v>
+        <v>28</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>399</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
       <c r="E13" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1">
       <c r="A14" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>32</v>
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
       <c r="E14" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1">
       <c r="A15" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>360</v>
+        <v>33</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>399</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
@@ -2359,7 +2413,7 @@
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="28" t="b">
         <v>0</v>
@@ -2367,28 +2421,28 @@
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1">
       <c r="A17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>38</v>
       </c>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
       <c r="A18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>41</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
@@ -2396,10 +2450,10 @@
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1">
       <c r="A19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="28" t="s">
         <v>42</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>43</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
@@ -2407,13 +2461,13 @@
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
       <c r="A20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>45</v>
-      </c>
       <c r="C20" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="39"/>
@@ -2427,10 +2481,10 @@
     </row>
     <row r="22" spans="1:5" s="23" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="86" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
@@ -2438,10 +2492,10 @@
     </row>
     <row r="23" spans="1:5" s="23" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="86" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
@@ -2449,10 +2503,10 @@
     </row>
     <row r="24" spans="1:5" s="23" customFormat="1" ht="14.25" customHeight="1">
       <c r="A24" s="86" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
@@ -2460,7 +2514,7 @@
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1">
       <c r="A25" s="88" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="89"/>
       <c r="C25" s="89"/>
@@ -2483,7 +2537,7 @@
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="28" t="b">
         <v>1</v>
@@ -2493,12 +2547,12 @@
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="45" t="str">
         <f>IF(B9="English",LanguageSettings!$B2,IF(B9="Spanish",LanguageSettings!$D2,LanguageSettings!$C2))</f>
@@ -2507,7 +2561,7 @@
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
       <c r="E29" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1">
@@ -2518,7 +2572,7 @@
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1">
       <c r="A31" s="88" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" s="89"/>
       <c r="C31" s="89"/>
@@ -2527,70 +2581,70 @@
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>52</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>53</v>
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
       <c r="E32" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1">
       <c r="A33" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="30" t="s">
         <v>55</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>56</v>
       </c>
       <c r="C33" s="47"/>
       <c r="D33" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="39" t="s">
         <v>56</v>
-      </c>
-      <c r="E33" s="39" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1">
       <c r="A34" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="47"/>
       <c r="D34" s="42"/>
       <c r="E34" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1">
       <c r="A35" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="47"/>
       <c r="D35" s="42"/>
       <c r="E35" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1">
       <c r="A36" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="42"/>
       <c r="E36" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="28" t="b">
         <v>0</v>
@@ -2598,51 +2652,51 @@
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
       <c r="E37" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1">
       <c r="A38" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
       <c r="D38" s="28"/>
       <c r="E38" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1">
       <c r="A39" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>
       <c r="E39" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1">
       <c r="A40" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="C40" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="D40" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40" s="38" t="s">
         <v>72</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1">
       <c r="A41" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="45">
         <v>25</v>
@@ -2650,12 +2704,12 @@
       <c r="C41" s="45"/>
       <c r="D41" s="45"/>
       <c r="E41" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1">
       <c r="A42" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
@@ -2668,10 +2722,10 @@
     </row>
     <row r="44" spans="1:5" ht="15.6" customHeight="1">
       <c r="A44" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="48" t="s">
         <v>77</v>
-      </c>
-      <c r="B44" s="48" t="s">
-        <v>78</v>
       </c>
       <c r="C44" s="30"/>
       <c r="D44" s="30"/>
@@ -2679,15 +2733,15 @@
     </row>
     <row r="45" spans="1:5" ht="13.95" customHeight="1">
       <c r="A45" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="30" t="s">
         <v>79</v>
-      </c>
-      <c r="B45" s="30" t="s">
-        <v>80</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
       <c r="E45" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.95" customHeight="1">
@@ -2696,7 +2750,7 @@
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1">
       <c r="A47" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="28" t="b">
         <v>1</v>
@@ -2709,7 +2763,7 @@
     </row>
     <row r="48" spans="1:5" ht="14.25" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" s="30" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B3,IF(B9="Spanish",LanguageSettings!$D3,LanguageSettings!$C3)),"%ProcessName%",B3)</f>
@@ -2724,12 +2778,12 @@
         <v>INT - SENICO - Factures fournisseurs - Status Report</v>
       </c>
       <c r="E48" s="38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="13.95" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B49" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B4,IF(B9="Spanish",LanguageSettings!$D4,LanguageSettings!$C4))</f>
@@ -2739,12 +2793,12 @@
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
       <c r="E49" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="14.25" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B5,IF(B9="Spanish",LanguageSettings!$D5,LanguageSettings!$C5))</f>
@@ -2753,12 +2807,12 @@
       <c r="C50" s="30"/>
       <c r="D50" s="30"/>
       <c r="E50" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13.95" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B6,IF(B9="Spanish",LanguageSettings!$D6,LanguageSettings!$C6))</f>
@@ -2767,12 +2821,12 @@
       <c r="C51" s="47"/>
       <c r="D51" s="42"/>
       <c r="E51" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.25" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B7,IF(B9="Spanish",LanguageSettings!$D7,LanguageSettings!$C7))</f>
@@ -2781,53 +2835,53 @@
       <c r="C52" s="30"/>
       <c r="D52" s="30"/>
       <c r="E52" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="14.25" customHeight="1">
       <c r="A53" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B53" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="34" t="s">
+      <c r="D53" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E53" s="39" t="s">
         <v>94</v>
-      </c>
-      <c r="D53" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E53" s="39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="14.25" customHeight="1">
       <c r="A54" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="30" t="s">
         <v>96</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>97</v>
       </c>
       <c r="C54" s="30"/>
       <c r="D54" s="30"/>
       <c r="E54" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
       <c r="E55" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="14.25" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B56" s="30">
         <v>3</v>
@@ -2835,7 +2889,7 @@
       <c r="C56" s="30"/>
       <c r="D56" s="30"/>
       <c r="E56" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="14.25" customHeight="1">
@@ -2847,46 +2901,46 @@
     </row>
     <row r="58" spans="1:5" ht="14.25" customHeight="1">
       <c r="A58" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="30" t="s">
         <v>103</v>
-      </c>
-      <c r="B58" s="30" t="s">
-        <v>104</v>
       </c>
       <c r="C58" s="30"/>
       <c r="D58" s="30"/>
       <c r="E58" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="14.25" customHeight="1">
       <c r="A59" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="30" t="s">
         <v>106</v>
-      </c>
-      <c r="B59" s="30" t="s">
-        <v>107</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
       <c r="E59" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="14.25" customHeight="1">
       <c r="A60" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="30" t="s">
         <v>109</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>110</v>
       </c>
       <c r="C60" s="30"/>
       <c r="D60" s="30"/>
       <c r="E60" s="38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="14.25" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B61" s="28" t="b">
         <v>0</v>
@@ -2894,20 +2948,20 @@
       <c r="C61" s="30"/>
       <c r="D61" s="30"/>
       <c r="E61" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="14.25" customHeight="1">
       <c r="A62" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="28" t="s">
         <v>114</v>
-      </c>
-      <c r="B62" s="28" t="s">
-        <v>115</v>
       </c>
       <c r="C62" s="30"/>
       <c r="D62" s="30"/>
       <c r="E62" s="38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="14.25" customHeight="1">
@@ -2919,7 +2973,7 @@
     </row>
     <row r="64" spans="1:5" ht="14.25" customHeight="1">
       <c r="A64" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B64" s="28" t="b">
         <v>1</v>
@@ -2932,7 +2986,7 @@
     </row>
     <row r="65" spans="1:5" ht="14.25" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="30" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B10,IF(B9="Spanish",LanguageSettings!$D10,LanguageSettings!$C10)),"%ProcessName%",B3)</f>
@@ -2947,12 +3001,12 @@
         <v>INT - SENICO - Factures fournisseurs - System Exception</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="14.25" customHeight="1">
       <c r="A66" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B66" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B11,IF(B9="Spanish",LanguageSettings!$D11,LanguageSettings!$C11))</f>
@@ -2961,12 +3015,12 @@
       <c r="C66" s="30"/>
       <c r="D66" s="30"/>
       <c r="E66" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="14.25" customHeight="1">
       <c r="A67" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B67" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B12,IF(B9="Spanish",LanguageSettings!$D12,LanguageSettings!$C12))</f>
@@ -2976,48 +3030,48 @@
       <c r="C67" s="30"/>
       <c r="D67" s="30"/>
       <c r="E67" s="39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="14.25" customHeight="1">
       <c r="A68" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E68" s="39" t="s">
         <v>124</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C68" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D68" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E68" s="39" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="14.25" customHeight="1">
       <c r="A69" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C69" s="50"/>
       <c r="D69" s="50"/>
       <c r="E69" s="39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="14.25" customHeight="1">
       <c r="A70" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B70" s="50"/>
       <c r="C70" s="50"/>
       <c r="D70" s="50"/>
       <c r="E70" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="14.25" customHeight="1">
@@ -3028,7 +3082,7 @@
     </row>
     <row r="72" spans="1:5" ht="14.25" customHeight="1">
       <c r="A72" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B72" s="28" t="b">
         <v>1</v>
@@ -3041,7 +3095,7 @@
     </row>
     <row r="73" spans="1:5" ht="14.25" customHeight="1">
       <c r="A73" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B73" s="30" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B13,IF(B9="Spanish",LanguageSettings!$D13,LanguageSettings!$C13)),"%ProcessName%",B3)</f>
@@ -3056,12 +3110,12 @@
         <v>INT - SENICO - Factures fournisseurs - Casier judiciaire non lisible par le robot pour le collaborateur %COLLABORATEUR% , Matricule : %MATRICULE% - Business Rule Exception</v>
       </c>
       <c r="E73" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="14.25" customHeight="1">
       <c r="A74" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B74" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B14,IF(B9="Spanish",LanguageSettings!$D14,LanguageSettings!$C14))</f>
@@ -3074,43 +3128,43 @@
     </row>
     <row r="75" spans="1:5" ht="14.25" customHeight="1">
       <c r="A75" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B75" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E75" s="39" t="s">
         <v>134</v>
-      </c>
-      <c r="B75" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C75" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D75" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E75" s="39" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="14.25" customHeight="1">
       <c r="A76" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" t="s">
         <v>136</v>
-      </c>
-      <c r="B76" t="s">
-        <v>137</v>
       </c>
       <c r="C76" s="28"/>
       <c r="D76" s="28"/>
       <c r="E76" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="14.25" customHeight="1">
       <c r="A77" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B77" s="28"/>
       <c r="C77" s="28"/>
       <c r="D77" s="28"/>
       <c r="E77" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="14.25" customHeight="1">
@@ -3122,7 +3176,7 @@
     </row>
     <row r="79" spans="1:5" ht="14.25" customHeight="1">
       <c r="A79" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B79" s="28" t="b">
         <v>0</v>
@@ -3132,12 +3186,12 @@
       </c>
       <c r="D79" s="28"/>
       <c r="E79" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="14.25" customHeight="1">
       <c r="A80" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B80" s="30" t="str">
         <f>SUBSTITUTE(IF(B9="English",LanguageSettings!$B8,IF(B9="Spanish",LanguageSettings!$D8,LanguageSettings!$C8)),"%Process%",B3)</f>
@@ -3152,12 +3206,12 @@
         <v>INT - SENICO - Factures fournisseurs - Process Started</v>
       </c>
       <c r="E80" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="14.25" customHeight="1">
       <c r="A81" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B81" s="30" t="str">
         <f>IF(B9="English",LanguageSettings!$B9,IF(B9="Spanish",LanguageSettings!$D9,LanguageSettings!$C9))</f>
@@ -3166,48 +3220,48 @@
       <c r="C81" s="30"/>
       <c r="D81" s="30"/>
       <c r="E81" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="14.25" customHeight="1">
       <c r="A82" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B82" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C82" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E82" s="39" t="s">
         <v>147</v>
-      </c>
-      <c r="B82" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C82" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D82" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E82" s="39" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="14.25" customHeight="1">
       <c r="A83" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C83" s="28"/>
       <c r="D83" s="28"/>
       <c r="E83" s="39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="14.25" customHeight="1">
       <c r="A84" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B84" s="30"/>
       <c r="C84" s="28"/>
       <c r="D84" s="28"/>
       <c r="E84" s="39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -3215,6 +3269,99 @@
       <c r="C85" s="25"/>
       <c r="D85" s="25"/>
       <c r="E85" s="37"/>
+    </row>
+    <row r="86" spans="1:5" ht="15" customHeight="1">
+      <c r="A86" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="B86" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="C86" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" s="28"/>
+      <c r="E86" s="38"/>
+    </row>
+    <row r="87" spans="1:5" ht="15" customHeight="1">
+      <c r="A87" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="B87" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="C87" s="30" t="str">
+        <f>"DEV - SENICO - Factures Fournisseurs - Compte Rendu"</f>
+        <v>DEV - SENICO - Factures Fournisseurs - Compte Rendu</v>
+      </c>
+      <c r="D87" s="30" t="str">
+        <f>"INT - "&amp;SUBSTITUTE(IF(B48="English",LanguageSettings!$B42,IF(B48="Spanish",LanguageSettings!$D42,LanguageSettings!$C42)),"%ProcessName%",B42)</f>
+        <v xml:space="preserve">INT - </v>
+      </c>
+      <c r="E87" s="38" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15" customHeight="1">
+      <c r="A88" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="B88" s="97" t="s">
+        <v>416</v>
+      </c>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="38" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15" customHeight="1">
+      <c r="A89" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="B89" s="97" t="s">
+        <v>415</v>
+      </c>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="38" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15" customHeight="1">
+      <c r="A90" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="B90" s="34"/>
+      <c r="C90" s="34" t="s">
+        <v>406</v>
+      </c>
+      <c r="D90" s="34"/>
+      <c r="E90" s="39" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15" customHeight="1">
+      <c r="A91" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="B91" s="30"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="38" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15" customHeight="1">
+      <c r="A92" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="B92" s="30"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="38" t="s">
+        <v>414</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3228,9 +3375,10 @@
     <hyperlink ref="C75" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C82" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C53" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C90" r:id="rId5" xr:uid="{97663257-540A-4CAF-897C-379F72ADE36A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <headerFooter>
     <oddFooter>&amp;C
 &amp;1#&amp;"verdana"&amp;8&amp;K282D87 RESTREINT</oddFooter>
@@ -3254,7 +3402,7 @@
           <x14:formula1>
             <xm:f>DataValidation!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B16:D16 B28:D28 B37:D37 B47:D47 B64:D64 B72:D72</xm:sqref>
+          <xm:sqref>B16:D16 B28:D28 B37:D37 B47:D47 B64:D64 B72:D72 B86:D86</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -3273,18 +3421,18 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41.21875" style="82" customWidth="1"/>
-    <col min="2" max="2" width="71.44140625" style="82" customWidth="1"/>
-    <col min="3" max="3" width="60.5546875" style="78" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" style="78" customWidth="1"/>
-    <col min="5" max="5" width="214.21875" style="72" customWidth="1"/>
-    <col min="6" max="16384" width="14.44140625" style="65"/>
+    <col min="1" max="1" width="41.20703125" style="82" customWidth="1"/>
+    <col min="2" max="2" width="71.41796875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="60.5234375" style="78" customWidth="1"/>
+    <col min="4" max="4" width="36.68359375" style="78" customWidth="1"/>
+    <col min="5" max="5" width="214.20703125" style="72" customWidth="1"/>
+    <col min="6" max="16384" width="14.41796875" style="65"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="56" customFormat="1" ht="15.6" customHeight="1">
@@ -3306,7 +3454,7 @@
     </row>
     <row r="2" spans="1:14" s="60" customFormat="1" ht="15.6" customHeight="1">
       <c r="A2" s="57" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B2" s="58"/>
       <c r="C2" s="58"/>
@@ -3315,15 +3463,15 @@
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1">
       <c r="A3" s="61" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>153</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>154</v>
       </c>
       <c r="C3" s="63"/>
       <c r="D3" s="63"/>
       <c r="E3" s="64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" s="63"/>
       <c r="G3" s="63"/>
@@ -3337,15 +3485,15 @@
     </row>
     <row r="4" spans="1:14" ht="14.25" customHeight="1">
       <c r="A4" s="61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="62" t="s">
         <v>156</v>
-      </c>
-      <c r="B4" s="62" t="s">
-        <v>157</v>
       </c>
       <c r="C4" s="63"/>
       <c r="D4" s="63"/>
       <c r="E4" s="64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" s="63"/>
       <c r="G4" s="63"/>
@@ -3359,15 +3507,15 @@
     </row>
     <row r="5" spans="1:14" ht="14.25" customHeight="1">
       <c r="A5" s="61" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" s="63"/>
       <c r="D5" s="63"/>
       <c r="E5" s="64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F5" s="63"/>
       <c r="G5" s="63"/>
@@ -3381,7 +3529,7 @@
     </row>
     <row r="6" spans="1:14" s="70" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="66" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -3390,17 +3538,17 @@
     </row>
     <row r="7" spans="1:14" ht="14.25" customHeight="1">
       <c r="A7" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="62" t="s">
         <v>159</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>160</v>
       </c>
       <c r="C7" s="63"/>
       <c r="D7" s="63"/>
     </row>
     <row r="8" spans="1:14" ht="14.25" customHeight="1">
       <c r="A8" s="71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="62">
         <v>20</v>
@@ -3410,101 +3558,101 @@
     </row>
     <row r="9" spans="1:14" ht="14.25" customHeight="1">
       <c r="A9" s="71" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C9" s="63"/>
       <c r="D9" s="63"/>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1">
       <c r="A10" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>164</v>
-      </c>
       <c r="C10" s="63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" s="63"/>
     </row>
     <row r="11" spans="1:14" ht="14.25" customHeight="1">
       <c r="A11" s="71" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>166</v>
-      </c>
       <c r="C11" s="63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11" s="63"/>
     </row>
     <row r="12" spans="1:14" ht="14.25" customHeight="1">
       <c r="A12" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="62" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>168</v>
-      </c>
       <c r="C12" s="63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D12" s="63"/>
     </row>
     <row r="13" spans="1:14" ht="14.25" customHeight="1">
       <c r="A13" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="62" t="s">
-        <v>170</v>
-      </c>
       <c r="C13" s="63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D13" s="63"/>
     </row>
     <row r="14" spans="1:14" ht="14.25" customHeight="1">
       <c r="A14" s="71" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="B14" s="73" t="s">
-        <v>172</v>
-      </c>
       <c r="C14" s="65" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" s="63"/>
     </row>
     <row r="15" spans="1:14" ht="14.25" customHeight="1">
       <c r="A15" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="73" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="73" t="s">
-        <v>174</v>
-      </c>
       <c r="C15" s="65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15" s="63"/>
     </row>
     <row r="16" spans="1:14" ht="14.25" customHeight="1">
       <c r="A16" s="71" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="73" t="s">
         <v>175</v>
       </c>
-      <c r="B16" s="73" t="s">
-        <v>176</v>
-      </c>
       <c r="C16" s="65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D16" s="63"/>
     </row>
     <row r="17" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="66" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B17" s="67"/>
       <c r="C17" s="68"/>
@@ -3513,79 +3661,79 @@
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
       <c r="A18" s="71" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="73" t="s">
         <v>177</v>
-      </c>
-      <c r="B18" s="73" t="s">
-        <v>178</v>
       </c>
       <c r="C18" s="65"/>
       <c r="D18" s="63"/>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1">
       <c r="A19" s="71" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="73" t="s">
         <v>179</v>
-      </c>
-      <c r="B19" s="73" t="s">
-        <v>180</v>
       </c>
       <c r="C19" s="65"/>
       <c r="D19" s="63"/>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
       <c r="A20" s="71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B20" s="73" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C20" s="65"/>
       <c r="D20" s="63"/>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1">
       <c r="A21" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="B21" s="73" t="s">
         <v>351</v>
-      </c>
-      <c r="B21" s="73" t="s">
-        <v>352</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="63"/>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1">
       <c r="A22" s="71" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B22" s="73" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C22" s="65"/>
       <c r="D22" s="63"/>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
       <c r="A23" s="71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C23" s="65"/>
       <c r="D23" s="63"/>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1">
       <c r="A24" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="B24" s="73" t="s">
-        <v>183</v>
-      </c>
       <c r="C24" s="65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D24" s="63"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1">
       <c r="A25" s="71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B25" s="73">
         <v>0.5</v>
@@ -3597,137 +3745,137 @@
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1">
       <c r="A26" s="71" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="75" t="s">
         <v>192</v>
       </c>
-      <c r="B26" s="75" t="s">
-        <v>193</v>
-      </c>
       <c r="C26" s="76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D26" s="63"/>
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1">
       <c r="A27" s="71" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="B27" s="73" t="s">
-        <v>195</v>
-      </c>
       <c r="C27" s="65" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D27" s="63"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="71" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="B28" s="75" t="s">
-        <v>197</v>
-      </c>
       <c r="C28" s="76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D28" s="63"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="71" t="s">
+        <v>197</v>
+      </c>
+      <c r="B29" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="B29" s="73" t="s">
-        <v>199</v>
-      </c>
       <c r="C29" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D29" s="63"/>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1">
       <c r="A30" s="71" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B30" s="73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D30" s="63"/>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1">
       <c r="A31" s="84" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B31" s="83" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="63"/>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1">
       <c r="A32" s="84" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B32" s="83" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="63"/>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1">
       <c r="A33" s="84" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B33" s="83" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C33" s="65"/>
       <c r="D33" s="63"/>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1">
       <c r="A34" s="84" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B34" s="83" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C34" s="65"/>
       <c r="D34" s="63"/>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1">
       <c r="A35" s="84" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B35" s="73" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C35" s="65"/>
       <c r="D35" s="63"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1">
       <c r="A36" s="84" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B36" s="73" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C36" s="65"/>
       <c r="D36" s="63"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1">
       <c r="A37" s="84" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B37" s="73" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C37" s="65"/>
       <c r="D37" s="63"/>
     </row>
     <row r="38" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
       <c r="A38" s="66" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B38" s="67"/>
       <c r="C38" s="68"/>
@@ -3736,118 +3884,118 @@
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1">
       <c r="A39" s="71" t="s">
+        <v>352</v>
+      </c>
+      <c r="B39" s="73" t="s">
         <v>353</v>
       </c>
-      <c r="B39" s="73" t="s">
-        <v>354</v>
-      </c>
       <c r="C39" s="65" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D39" s="63"/>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1">
       <c r="A40" s="71" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B40" s="73" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C40" s="65"/>
       <c r="D40" s="63"/>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1">
       <c r="A41" s="71" t="s">
+        <v>354</v>
+      </c>
+      <c r="B41" s="73" t="s">
         <v>355</v>
-      </c>
-      <c r="B41" s="73" t="s">
-        <v>356</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="63"/>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1">
       <c r="A42" s="71" t="s">
+        <v>356</v>
+      </c>
+      <c r="B42" s="73" t="s">
         <v>357</v>
-      </c>
-      <c r="B42" s="73" t="s">
-        <v>358</v>
       </c>
       <c r="C42" s="65"/>
       <c r="D42" s="63"/>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1">
       <c r="A43" s="71" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B43" s="73" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C43" s="65"/>
       <c r="D43" s="63"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" customHeight="1">
       <c r="A44" s="71" t="s">
+        <v>185</v>
+      </c>
+      <c r="B44" s="73" t="s">
         <v>186</v>
       </c>
-      <c r="B44" s="73" t="s">
-        <v>187</v>
-      </c>
       <c r="C44" s="65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D44" s="63"/>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1">
       <c r="A45" s="71" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B45" s="73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D45" s="63"/>
     </row>
     <row r="46" spans="1:5" ht="14.25" customHeight="1">
       <c r="A46" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="B46" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="B46" s="73" t="s">
-        <v>190</v>
-      </c>
       <c r="C46" s="65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D46" s="63"/>
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1">
       <c r="A47" s="71" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B47" s="73" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C47" s="65"/>
       <c r="D47" s="63"/>
     </row>
     <row r="48" spans="1:5" ht="14.25" customHeight="1">
       <c r="A48" s="71" t="s">
+        <v>385</v>
+      </c>
+      <c r="B48" s="73" t="s">
         <v>387</v>
-      </c>
-      <c r="B48" s="73" t="s">
-        <v>389</v>
       </c>
       <c r="C48" s="65"/>
       <c r="D48" s="63"/>
       <c r="E48" s="72" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
       <c r="A49" s="66" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B49" s="67"/>
       <c r="C49" s="68"/>
@@ -3856,117 +4004,117 @@
     </row>
     <row r="50" spans="1:5" ht="13.2" customHeight="1">
       <c r="A50" s="71" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B50" s="77" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13.2" customHeight="1">
       <c r="A51" s="79" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B51" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13.2" customHeight="1">
       <c r="A52" s="79" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B52" s="80" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1">
       <c r="A53" s="71" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B53" s="62" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D53" s="63"/>
       <c r="E53" s="72" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1">
       <c r="A54" s="71" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B54" s="73" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D54" s="63"/>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1">
       <c r="A55" s="71" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B55" s="73" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D55" s="63"/>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1">
       <c r="A56" s="71" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B56" s="62" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D56" s="63"/>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1">
       <c r="A57" s="71" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B57" s="73" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D57" s="63"/>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1">
       <c r="A58" s="71" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B58" s="73" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D58" s="63"/>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1">
       <c r="A59" s="71" t="s">
+        <v>320</v>
+      </c>
+      <c r="B59" s="62" t="s">
         <v>321</v>
-      </c>
-      <c r="B59" s="62" t="s">
-        <v>322</v>
       </c>
       <c r="D59" s="63"/>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1">
       <c r="A60" s="71" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B60" s="73" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C60" s="62"/>
       <c r="D60" s="63"/>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1">
       <c r="A61" s="71" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B61" s="73" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C61" s="62"/>
       <c r="D61" s="63"/>
     </row>
     <row r="62" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
       <c r="A62" s="66" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B62" s="67"/>
       <c r="C62" s="68"/>
@@ -3975,27 +4123,27 @@
     </row>
     <row r="63" spans="1:5" ht="28.8">
       <c r="A63" s="71" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C63" s="63"/>
       <c r="D63" s="63"/>
     </row>
     <row r="64" spans="1:5" ht="72">
       <c r="A64" s="71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B64" s="62" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C64" s="63"/>
       <c r="D64" s="63"/>
     </row>
     <row r="65" spans="1:5" s="70" customFormat="1" ht="15" customHeight="1">
       <c r="A65" s="66" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B65" s="67"/>
       <c r="C65" s="68"/>
@@ -4004,20 +4152,20 @@
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1">
       <c r="A66" s="81" t="s">
+        <v>341</v>
+      </c>
+      <c r="B66" s="77" t="s">
         <v>342</v>
-      </c>
-      <c r="B66" s="77" t="s">
-        <v>343</v>
       </c>
       <c r="C66" s="63"/>
       <c r="D66" s="63"/>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1">
       <c r="A67" s="71" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B67" s="62" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C67" s="63"/>
       <c r="D67" s="63"/>
@@ -4203,13 +4351,13 @@
       <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="1"/>
-    <col min="2" max="2" width="48.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="143.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.20703125" customWidth="1"/>
+    <col min="2" max="2" width="48.20703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.41796875" customWidth="1"/>
+    <col min="4" max="4" width="14.20703125" customWidth="1"/>
+    <col min="5" max="5" width="143.41796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1">
@@ -4231,7 +4379,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="92"/>
       <c r="C2" s="92"/>
@@ -4240,7 +4388,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" s="19">
         <v>0</v>
@@ -4248,12 +4396,12 @@
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="3">
         <v>200</v>
@@ -4261,12 +4409,12 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -4274,12 +4422,12 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1">
       <c r="A6" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="15">
         <v>3</v>
@@ -4287,13 +4435,13 @@
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="19">
         <v>5</v>
@@ -4301,12 +4449,12 @@
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1">
       <c r="A9" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9" s="3">
         <v>30</v>
@@ -4314,12 +4462,12 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1">
       <c r="A10" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="15">
         <v>120</v>
@@ -4327,13 +4475,13 @@
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:5" ht="14.25" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="19">
         <v>1</v>
@@ -4341,12 +4489,12 @@
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" s="3">
         <v>15</v>
@@ -4354,12 +4502,12 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="15">
         <v>60</v>
@@ -4367,13 +4515,13 @@
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:5" ht="14.25" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B16" s="19">
         <v>0.6</v>
@@ -4381,12 +4529,12 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1">
       <c r="A17" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B17" s="3">
         <v>0.8</v>
@@ -4394,12 +4542,12 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B18" s="15">
         <v>0.9</v>
@@ -4407,92 +4555,92 @@
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
       <c r="A20" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>228</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>229</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1">
       <c r="A21" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1">
       <c r="A22" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
       <c r="A23" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>238</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1">
       <c r="A24" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B24" s="15" t="s">
         <v>240</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>241</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:5" ht="14.25" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B27" s="19">
         <v>0</v>
@@ -4500,12 +4648,12 @@
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
       <c r="E27" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -4513,12 +4661,12 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B29" s="15">
         <v>0</v>
@@ -4526,26 +4674,26 @@
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:5" ht="14.25" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
       <c r="E31" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.1" customHeight="1">
       <c r="A32" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B32" s="15">
         <v>7</v>
@@ -4553,13 +4701,13 @@
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.1" customHeight="1"/>
     <row r="34" spans="1:5" ht="14.1" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B34" s="19">
         <v>3</v>
@@ -4567,12 +4715,12 @@
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.1" customHeight="1">
       <c r="A35" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B35" s="15">
         <v>5</v>
@@ -4580,13 +4728,13 @@
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:5" ht="14.25" customHeight="1">
       <c r="A37" s="94" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B37" s="95"/>
       <c r="C37" s="95"/>
@@ -4595,7 +4743,7 @@
     </row>
     <row r="38" spans="1:5" s="17" customFormat="1" ht="14.25" customHeight="1">
       <c r="A38" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -4621,12 +4769,12 @@
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" customWidth="1"/>
-    <col min="3" max="4" width="31.21875" customWidth="1"/>
-    <col min="5" max="5" width="94.21875" customWidth="1"/>
+    <col min="2" max="2" width="31.5234375" customWidth="1"/>
+    <col min="3" max="4" width="31.20703125" customWidth="1"/>
+    <col min="5" max="5" width="94.20703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1">
@@ -4637,21 +4785,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4659,10 +4807,10 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4705,232 +4853,232 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="69.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.20703125" defaultRowHeight="69.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="50.5546875" customWidth="1"/>
-    <col min="2" max="5" width="50.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="50.5234375" customWidth="1"/>
+    <col min="2" max="5" width="50.5234375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4">
       <c r="A3" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="89.25" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>275</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="89.25" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>279</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="89.25" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="89.25" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>287</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.4">
       <c r="A8" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="89.25" customHeight="1">
       <c r="A9" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>291</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>292</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="14.4">
       <c r="A10" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="89.25" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>296</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="178.95" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2">
       <c r="A13" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>303</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="134.55000000000001" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>306</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="134.55000000000001" customHeight="1">
@@ -4957,43 +5105,43 @@
       <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.20703125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="32.5546875" customWidth="1"/>
+    <col min="1" max="2" width="14.5234375" customWidth="1"/>
+    <col min="3" max="3" width="32.5234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>0</v>
@@ -5002,20 +5150,20 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>